<commit_message>
Revised bom-sc with manufacturer information, description, and packaging
</commit_message>
<xml_diff>
--- a/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
+++ b/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="15" windowWidth="22755" windowHeight="9765"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="224">
   <si>
     <t>Item #</t>
   </si>
@@ -48,27 +48,6 @@
     <t>J11</t>
   </si>
   <si>
-    <t>I2C Header</t>
-  </si>
-  <si>
-    <t>Auxiliary Header</t>
-  </si>
-  <si>
-    <t>UART Header</t>
-  </si>
-  <si>
-    <t>BOOT0 Jumper</t>
-  </si>
-  <si>
-    <t>BOOT1 Jumper</t>
-  </si>
-  <si>
-    <t>PGOOD Jumper</t>
-  </si>
-  <si>
-    <t>Debug Header</t>
-  </si>
-  <si>
     <t>25 MHz</t>
   </si>
   <si>
@@ -81,9 +60,6 @@
     <t>BAT54</t>
   </si>
   <si>
-    <t>BQ24725QFN-20</t>
-  </si>
-  <si>
     <t>BSS138W-7-F</t>
   </si>
   <si>
@@ -141,18 +117,9 @@
     <t>DIODE-0603</t>
   </si>
   <si>
-    <t>FDS6680ASOIC8</t>
-  </si>
-  <si>
-    <t>4.7uH/IHLP2525CZER4R7M01</t>
-  </si>
-  <si>
     <t>KS8999</t>
   </si>
   <si>
-    <t>TBD/FB</t>
-  </si>
-  <si>
     <t>RGB</t>
   </si>
   <si>
@@ -243,21 +210,12 @@
     <t>10m/WSLP1206R0100FEA/1.0 Watt</t>
   </si>
   <si>
-    <t>SIS412DNSOP-8</t>
-  </si>
-  <si>
     <t>SMAJ18CA</t>
   </si>
   <si>
     <t>SN65220DBV</t>
   </si>
   <si>
-    <t>STM32F407V100-PIN_QFP</t>
-  </si>
-  <si>
-    <t>TPS2420QFN-16</t>
-  </si>
-  <si>
     <t>TPTP06R</t>
   </si>
   <si>
@@ -402,24 +360,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>1.27MM_HDR_1X3</t>
-  </si>
-  <si>
-    <t>1.27MM_HDR_1X4</t>
-  </si>
-  <si>
-    <t>1.27MM_HDR_1X4_TX_RX</t>
-  </si>
-  <si>
-    <t>1.27MM_HDR_2X12X1</t>
-  </si>
-  <si>
-    <t>1.27MM_HDR_2X5</t>
-  </si>
-  <si>
-    <t>8Y</t>
-  </si>
-  <si>
     <t>C-EU0402-B-NOSILK</t>
   </si>
   <si>
@@ -438,9 +378,6 @@
     <t>IHLP-2525CZ-01</t>
   </si>
   <si>
-    <t>L-BEAD-0603-B</t>
-  </si>
-  <si>
     <t>LED_RGB_PLCC-6</t>
   </si>
   <si>
@@ -568,6 +505,189 @@
   </si>
   <si>
     <t>U7,U8,U9,U10,U11,U12,U13</t>
+  </si>
+  <si>
+    <t>50 mil (1.27 mm) Inline 1x3 Male Header</t>
+  </si>
+  <si>
+    <t>50 mil (1.27 mm) Inline 1x4 Male Header</t>
+  </si>
+  <si>
+    <t>50 mil (1.27 mm) Inline 1x2 Male Header</t>
+  </si>
+  <si>
+    <t>50 mil (1.27 mm)  2x5 Male Header</t>
+  </si>
+  <si>
+    <t>8Y-25.000MEEQ-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EMI Filters 90 Ohms </t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>Pulse Transformers</t>
+  </si>
+  <si>
+    <t>ALT4532-201-T001</t>
+  </si>
+  <si>
+    <t>ACM2012-900-2P-T002</t>
+  </si>
+  <si>
+    <t>30 V Schottky barrier (double) diodes</t>
+  </si>
+  <si>
+    <t>Texas Instruments</t>
+  </si>
+  <si>
+    <t>20-pin QFN</t>
+  </si>
+  <si>
+    <t>2-4Cell Li+ Battery SMBus Charge Controller with N-Channel Power MOSFET Selector</t>
+  </si>
+  <si>
+    <t>SOT23</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Testpoint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET 50V 200mW </t>
+  </si>
+  <si>
+    <t>DIODES Inc</t>
+  </si>
+  <si>
+    <t>BQ24725RGRT</t>
+  </si>
+  <si>
+    <t>FDS6680A</t>
+  </si>
+  <si>
+    <t>MOSFET N-Channel 30V 12.5A</t>
+  </si>
+  <si>
+    <t>Fairchild Semiconductor</t>
+  </si>
+  <si>
+    <t>4.7 uH Low Profile, High Current IHLP</t>
+  </si>
+  <si>
+    <t>Micrel</t>
+  </si>
+  <si>
+    <t>Linear Technology</t>
+  </si>
+  <si>
+    <t>2A, 36V DC/DC Step-Down μModule Regulator</t>
+  </si>
+  <si>
+    <t>50 pin BLGA</t>
+  </si>
+  <si>
+    <t>LTM8023EV#PBF-ND</t>
+  </si>
+  <si>
+    <t>1A Low-Voltage uCap LDO</t>
+  </si>
+  <si>
+    <t>8-pin SOIC</t>
+  </si>
+  <si>
+    <t>ARM Cortex-M4 32b MCU+FPU, 210DMIPS, Ethernet</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>STM32F407V100</t>
+  </si>
+  <si>
+    <t>3-V to 20-V Integrated FET Hot Swap with Load Current Monitor</t>
+  </si>
+  <si>
+    <t>16-pin QFN</t>
+  </si>
+  <si>
+    <t>296-24175-1-ND</t>
+  </si>
+  <si>
+    <t>TPS2420</t>
+  </si>
+  <si>
+    <t>208-pin PQFP</t>
+  </si>
+  <si>
+    <t>100-pin LQFP</t>
+  </si>
+  <si>
+    <t>Transient Voltage Suppression Diode</t>
+  </si>
+  <si>
+    <t>Littlefuse Inc</t>
+  </si>
+  <si>
+    <t>DO-214AC, SMA</t>
+  </si>
+  <si>
+    <t>SMAJ18CALFCT-ND</t>
+  </si>
+  <si>
+    <t>SIS412DN-T1-GE3CT-ND</t>
+  </si>
+  <si>
+    <t>PowerPAK 1212-8</t>
+  </si>
+  <si>
+    <t>SiS412DN</t>
+  </si>
+  <si>
+    <t>Vishay Siliconix</t>
+  </si>
+  <si>
+    <t>N-Channel 30-V (D-S) MOSFET</t>
+  </si>
+  <si>
+    <t>BSS138W-FDICT-ND</t>
+  </si>
+  <si>
+    <t>296-27827-1-ND</t>
+  </si>
+  <si>
+    <t>576-1044-ND</t>
+  </si>
+  <si>
+    <t>USB Port Transient Suppressors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TXC Corp. </t>
+  </si>
+  <si>
+    <t>Non-Standard (Custom size)</t>
+  </si>
+  <si>
+    <t>Ferrite Bead</t>
+  </si>
+  <si>
+    <t>0.8 Ohm, Low-Voltage, 4-Channel Analog Multiplexer</t>
+  </si>
+  <si>
+    <t>Maxim IC</t>
+  </si>
+  <si>
+    <t>12-pin QFN</t>
+  </si>
+  <si>
+    <t>MAX4734ETC+-ND</t>
   </si>
 </sst>
 </file>
@@ -939,17 +1059,19 @@
   <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -994,13 +1116,13 @@
         <v>9</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>10</v>
+        <v>163</v>
       </c>
       <c r="H3" t="s">
-        <v>128</v>
+        <v>179</v>
       </c>
       <c r="I3" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1011,16 +1133,16 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>11</v>
+        <v>164</v>
       </c>
       <c r="H4" t="s">
-        <v>129</v>
+        <v>179</v>
       </c>
       <c r="I4" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1031,16 +1153,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>12</v>
+        <v>164</v>
       </c>
       <c r="H5" t="s">
-        <v>130</v>
+        <v>179</v>
       </c>
       <c r="I5" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1051,16 +1173,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>13</v>
+        <v>165</v>
       </c>
       <c r="H6" t="s">
+        <v>179</v>
+      </c>
+      <c r="I6" t="s">
         <v>131</v>
-      </c>
-      <c r="I6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1071,1351 +1193,1703 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>14</v>
+        <v>165</v>
       </c>
       <c r="H7" t="s">
+        <v>179</v>
+      </c>
+      <c r="I7" t="s">
         <v>131</v>
       </c>
-      <c r="I7" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>15</v>
+        <v>165</v>
       </c>
       <c r="H8" t="s">
+        <v>179</v>
+      </c>
+      <c r="I8" t="s">
         <v>131</v>
       </c>
-      <c r="I8" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="H9" t="s">
-        <v>132</v>
+        <v>179</v>
       </c>
       <c r="I9" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>73</v>
+      </c>
+      <c r="D10" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" t="s">
+        <v>167</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>133</v>
+        <v>178</v>
       </c>
       <c r="I10" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
       <c r="B11">
         <v>16</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>150</v>
+        <v>129</v>
+      </c>
+      <c r="D11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" t="s">
+        <v>172</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>18</v>
+        <v>168</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
       <c r="B12">
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>149</v>
+        <v>128</v>
+      </c>
+      <c r="D12" t="s">
+        <v>169</v>
+      </c>
+      <c r="E12" t="s">
+        <v>171</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>19</v>
+        <v>170</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>74</v>
+      </c>
+      <c r="D13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>20</v>
+        <v>173</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
+        <v>177</v>
       </c>
       <c r="I13" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>21</v>
+        <v>75</v>
+      </c>
+      <c r="D14" t="s">
+        <v>174</v>
+      </c>
+      <c r="E14" t="s">
+        <v>183</v>
+      </c>
+      <c r="F14" t="s">
+        <v>214</v>
+      </c>
+      <c r="G14" t="s">
+        <v>176</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>175</v>
       </c>
       <c r="I14" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>76</v>
+      </c>
+      <c r="D15" t="s">
+        <v>182</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>213</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
       <c r="H15" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
       <c r="B16">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I17" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H18" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I18" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
       <c r="B19">
         <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H19" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I19" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I20" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I21" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H22" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I22" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
       <c r="B23">
         <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H23" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I23" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H24" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>23</v>
+      </c>
       <c r="B25">
         <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H25" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I25" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>24</v>
+      </c>
       <c r="B26">
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="H26" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="I26" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>25</v>
+      </c>
       <c r="B27">
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H27" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="I27" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>26</v>
+      </c>
       <c r="B28">
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H28" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="I28" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>27</v>
+      </c>
       <c r="B29">
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="H29" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="I29" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>28</v>
+      </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H30" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="I30" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H31" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="I31" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>30</v>
+      </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H32" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="I32" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>31</v>
+      </c>
       <c r="B33">
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H33" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="I33" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>32</v>
+      </c>
       <c r="B34">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="H34" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="I34" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>33</v>
+      </c>
       <c r="B35">
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>164</v>
+        <v>143</v>
+      </c>
+      <c r="D35" t="s">
+        <v>186</v>
+      </c>
+      <c r="E35" t="s">
+        <v>184</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>41</v>
+        <v>185</v>
       </c>
       <c r="H35" t="s">
-        <v>41</v>
+        <v>194</v>
       </c>
       <c r="I35" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>34</v>
+      </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>99</v>
+        <v>85</v>
+      </c>
+      <c r="D36" t="s">
+        <v>211</v>
+      </c>
+      <c r="E36" t="s">
+        <v>119</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>42</v>
+        <v>187</v>
       </c>
       <c r="H36" t="s">
-        <v>139</v>
+        <v>218</v>
       </c>
       <c r="I36" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>100</v>
+        <v>86</v>
+      </c>
+      <c r="D37" t="s">
+        <v>188</v>
+      </c>
+      <c r="E37" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" t="s">
+        <v>215</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H37" t="s">
-        <v>43</v>
+        <v>202</v>
       </c>
       <c r="I37" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>36</v>
+      </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H38" t="s">
-        <v>140</v>
+        <v>219</v>
+      </c>
+      <c r="H38">
+        <v>603</v>
       </c>
       <c r="I38" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>37</v>
+      </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="H39" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="I39" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>38</v>
+      </c>
       <c r="B40">
         <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="H40" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="I40" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>39</v>
+      </c>
       <c r="B41">
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H41" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="I41" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>40</v>
+      </c>
       <c r="B42">
         <v>7</v>
       </c>
       <c r="C42" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H42" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="I42" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>41</v>
+      </c>
       <c r="B43">
         <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="H43" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="I43" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>42</v>
+      </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>103</v>
+        <v>89</v>
+      </c>
+      <c r="D44" t="s">
+        <v>189</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" t="s">
+        <v>192</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>49</v>
+        <v>190</v>
       </c>
       <c r="H44" t="s">
-        <v>49</v>
+        <v>191</v>
       </c>
       <c r="I44" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>43</v>
+      </c>
       <c r="B45">
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>169</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>50</v>
+        <v>148</v>
+      </c>
+      <c r="D45" t="s">
+        <v>221</v>
+      </c>
+      <c r="E45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F45" t="s">
+        <v>223</v>
+      </c>
+      <c r="G45" t="s">
+        <v>220</v>
       </c>
       <c r="H45" t="s">
-        <v>50</v>
+        <v>222</v>
       </c>
       <c r="I45" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>44</v>
+      </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>104</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>51</v>
+        <v>90</v>
+      </c>
+      <c r="D46" t="s">
+        <v>188</v>
+      </c>
+      <c r="E46" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" t="s">
+        <v>193</v>
       </c>
       <c r="H46" t="s">
-        <v>51</v>
+        <v>194</v>
       </c>
       <c r="I46" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>45</v>
+      </c>
       <c r="B47">
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="H47" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="I47" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>46</v>
+      </c>
       <c r="B48">
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="H48" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="I48" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>47</v>
+      </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H49" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="I49" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>48</v>
+      </c>
       <c r="B50">
         <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="H50" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="I50" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>49</v>
+      </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H51" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I51" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>50</v>
+      </c>
       <c r="B52">
         <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="G52" s="5">
         <v>0</v>
       </c>
       <c r="H52" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I52" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
       <c r="B53">
         <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="H53" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I53" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="H54" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I54" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
       <c r="B55">
         <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="H55" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I55" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
       <c r="B56">
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="H56" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I56" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
       <c r="B57">
         <v>1</v>
       </c>
       <c r="C57" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="H57" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I57" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="H58" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I58" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
       <c r="B59">
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="H59" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I59" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
       <c r="B60">
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="H60" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I60" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
       <c r="B61">
         <v>24</v>
       </c>
       <c r="C61" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="H61" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I61" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="H62" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I62" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
       <c r="B63">
         <v>48</v>
       </c>
       <c r="C63" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="G63" s="5">
         <v>51</v>
       </c>
       <c r="H63" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I63" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="H64" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I64" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="G65" s="5">
         <v>100</v>
       </c>
       <c r="H65" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I65" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="G66" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H66" t="s">
+        <v>125</v>
+      </c>
+      <c r="I66" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>102</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H67" t="s">
+        <v>125</v>
+      </c>
+      <c r="I67" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>103</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H68" t="s">
+        <v>125</v>
+      </c>
+      <c r="I68" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>104</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H69" t="s">
+        <v>125</v>
+      </c>
+      <c r="I69" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
         <v>68</v>
       </c>
-      <c r="H66" t="s">
-        <v>146</v>
-      </c>
-      <c r="I66" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67" t="s">
-        <v>116</v>
-      </c>
-      <c r="G67" s="5" t="s">
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>105</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H70" t="s">
+        <v>125</v>
+      </c>
+      <c r="I70" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71">
         <v>69</v>
       </c>
-      <c r="H67" t="s">
-        <v>146</v>
-      </c>
-      <c r="I67" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68" t="s">
-        <v>117</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H68" t="s">
-        <v>146</v>
-      </c>
-      <c r="I68" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69" t="s">
-        <v>118</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="H69" t="s">
-        <v>146</v>
-      </c>
-      <c r="I69" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B70">
-        <v>1</v>
-      </c>
-      <c r="C70" t="s">
-        <v>119</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H70" t="s">
-        <v>146</v>
-      </c>
-      <c r="I70" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71">
         <v>27</v>
       </c>
       <c r="C71" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="G71" s="5">
         <v>750</v>
       </c>
       <c r="H71" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I71" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
       <c r="B72">
         <v>21</v>
       </c>
       <c r="C72" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="H72" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I72" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
       <c r="B73">
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="G73" s="5">
         <v>7.5</v>
       </c>
       <c r="H73" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="I73" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
       <c r="B74">
         <v>1</v>
       </c>
       <c r="C74" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="G74" s="5">
         <v>10</v>
       </c>
       <c r="H74" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
       <c r="I74" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
       <c r="B75">
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="G75" s="5">
         <v>2</v>
       </c>
       <c r="H75" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="I75" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
       <c r="B76">
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="H76" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="I76" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
       <c r="B77">
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="H77" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="I77" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
       <c r="B78">
         <v>2</v>
       </c>
       <c r="C78" t="s">
-        <v>181</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>75</v>
+        <v>160</v>
+      </c>
+      <c r="D78" t="s">
+        <v>211</v>
+      </c>
+      <c r="E78" t="s">
+        <v>210</v>
+      </c>
+      <c r="F78" t="s">
+        <v>208</v>
+      </c>
+      <c r="G78" t="s">
+        <v>212</v>
       </c>
       <c r="H78" t="s">
-        <v>75</v>
+        <v>209</v>
       </c>
       <c r="I78" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
       <c r="B79">
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>125</v>
-      </c>
-      <c r="G79" s="5" t="s">
-        <v>76</v>
+        <v>111</v>
+      </c>
+      <c r="D79" t="s">
+        <v>205</v>
+      </c>
+      <c r="E79" t="s">
+        <v>64</v>
+      </c>
+      <c r="F79" t="s">
+        <v>207</v>
+      </c>
+      <c r="G79" t="s">
+        <v>204</v>
       </c>
       <c r="H79" t="s">
-        <v>76</v>
+        <v>206</v>
       </c>
       <c r="I79" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
       <c r="B80">
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>126</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="H80" t="s">
-        <v>77</v>
+        <v>112</v>
+      </c>
+      <c r="D80" t="s">
+        <v>174</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G80" t="s">
+        <v>216</v>
       </c>
       <c r="I80" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
       <c r="B81">
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>127</v>
-      </c>
-      <c r="G81" s="5" t="s">
-        <v>78</v>
+        <v>113</v>
+      </c>
+      <c r="D81" t="s">
+        <v>196</v>
+      </c>
+      <c r="E81" t="s">
+        <v>197</v>
+      </c>
+      <c r="G81" t="s">
+        <v>195</v>
       </c>
       <c r="H81" t="s">
-        <v>78</v>
+        <v>203</v>
       </c>
       <c r="I81" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
       <c r="B82">
         <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>183</v>
-      </c>
-      <c r="G82" s="5" t="s">
-        <v>79</v>
+        <v>162</v>
+      </c>
+      <c r="D82" t="s">
+        <v>174</v>
+      </c>
+      <c r="E82" t="s">
+        <v>201</v>
+      </c>
+      <c r="F82" t="s">
+        <v>200</v>
+      </c>
+      <c r="G82" t="s">
+        <v>198</v>
       </c>
       <c r="H82" t="s">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="I82" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
       <c r="B83">
         <v>40</v>
       </c>
       <c r="C83" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="H83" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I83" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G84" s="5"/>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G85" s="5"/>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G86" s="5"/>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G87" s="5"/>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G88" s="5"/>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G89" s="5"/>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G90" s="5"/>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G91" s="5"/>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G92" s="5"/>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G93" s="5"/>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G94" s="5"/>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G95" s="5"/>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G96" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added recommended digikey part order to bom-sc
</commit_message>
<xml_diff>
--- a/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
+++ b/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="229">
   <si>
     <t>Item #</t>
   </si>
@@ -694,6 +694,15 @@
   </si>
   <si>
     <t>MOSFET P-CH 50V 130MA</t>
+  </si>
+  <si>
+    <t>FDS6680ACT-ND</t>
+  </si>
+  <si>
+    <t>576-1758-5-ND</t>
+  </si>
+  <si>
+    <t>497-11605-ND</t>
   </si>
 </sst>
 </file>
@@ -1066,8 +1075,8 @@
   <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,6 +1819,9 @@
       <c r="E35" t="s">
         <v>182</v>
       </c>
+      <c r="F35" t="s">
+        <v>226</v>
+      </c>
       <c r="G35" s="5" t="s">
         <v>183</v>
       </c>
@@ -2069,6 +2081,9 @@
       <c r="E46" t="s">
         <v>40</v>
       </c>
+      <c r="F46" t="s">
+        <v>227</v>
+      </c>
       <c r="G46" t="s">
         <v>191</v>
       </c>
@@ -2807,6 +2822,9 @@
       </c>
       <c r="E81" t="s">
         <v>195</v>
+      </c>
+      <c r="F81" t="s">
+        <v>228</v>
       </c>
       <c r="G81" t="s">
         <v>193</v>

</xml_diff>

<commit_message>
Changed LED size from 0402 to 0603 and added parts in bom
</commit_message>
<xml_diff>
--- a/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
+++ b/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="235">
   <si>
     <t>Item #</t>
   </si>
@@ -123,15 +123,6 @@
     <t>RGB</t>
   </si>
   <si>
-    <t>AMBER</t>
-  </si>
-  <si>
-    <t>GREEN</t>
-  </si>
-  <si>
-    <t>RED</t>
-  </si>
-  <si>
     <t>LTM8023</t>
   </si>
   <si>
@@ -360,12 +351,6 @@
     <t>LED_RGB_PLCC-6</t>
   </si>
   <si>
-    <t>LEDCHIPLED_0603</t>
-  </si>
-  <si>
-    <t>LEDSML0603</t>
-  </si>
-  <si>
     <t>R-US_0402-B-NOSILK</t>
   </si>
   <si>
@@ -426,12 +411,6 @@
     <t>LED1,LED5,LED9,LED13,LED17,LED21,LED25,LED29,LED33</t>
   </si>
   <si>
-    <t>LED22,LED38</t>
-  </si>
-  <si>
-    <t>LED3,LED6,LED8,LED11,LED14,LED16,LED39</t>
-  </si>
-  <si>
     <t>LED2,LED4,LED7,LED10,LED12,LED15,LED18</t>
   </si>
   <si>
@@ -709,6 +688,39 @@
   </si>
   <si>
     <t>J10,J15,J16,J17,J18,J19,J20,J21</t>
+  </si>
+  <si>
+    <t>LED3,LED6,LED8,LED11,LED14,LED16,LED22,LED38,LED39</t>
+  </si>
+  <si>
+    <t>Kingbright Company LLC</t>
+  </si>
+  <si>
+    <t>LED 1.6X0.8MM 590NM YLW CLR</t>
+  </si>
+  <si>
+    <t>LED 1.6X0.8MM 570NM GRN CLR</t>
+  </si>
+  <si>
+    <t>LED 1.6X0.8MM 625NM RED CLR</t>
+  </si>
+  <si>
+    <t>754-1124-1-ND</t>
+  </si>
+  <si>
+    <t>754-1116-1-ND</t>
+  </si>
+  <si>
+    <t>754-1117-1-ND</t>
+  </si>
+  <si>
+    <t>APT1608EC</t>
+  </si>
+  <si>
+    <t>APT1608CGCK</t>
+  </si>
+  <si>
+    <t>APT1608SYCK</t>
   </si>
 </sst>
 </file>
@@ -1078,11 +1090,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,10 +1102,10 @@
     <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1138,13 +1150,13 @@
         <v>9</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="H3" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1152,19 +1164,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H4" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1172,19 +1184,19 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H5" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1195,16 +1207,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="H6" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="I6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1215,22 +1227,22 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="I7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1241,22 +1253,22 @@
         <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D8" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E8" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1267,22 +1279,22 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="E9" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="H9" t="s">
         <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1293,22 +1305,22 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="H10" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="I10" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1319,25 +1331,25 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D11" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E11" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="F11" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="G11" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="H11" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="I11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1348,25 +1360,25 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1377,16 +1389,16 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I13" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1397,16 +1409,16 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I14" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1417,16 +1429,16 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I15" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1437,16 +1449,16 @@
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>18</v>
       </c>
       <c r="H16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I16" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1457,16 +1469,16 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>19</v>
       </c>
       <c r="H17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I17" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1477,16 +1489,16 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I18" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1497,16 +1509,16 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>21</v>
       </c>
       <c r="H19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I19" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1517,16 +1529,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H20" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I20" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1537,16 +1549,16 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>23</v>
       </c>
       <c r="H21" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1557,16 +1569,16 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>24</v>
       </c>
       <c r="H22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I22" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1577,16 +1589,16 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H23" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1597,16 +1609,16 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I24" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1617,16 +1629,16 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I25" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1637,16 +1649,16 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>28</v>
       </c>
       <c r="H26" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I26" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1657,16 +1669,16 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>29</v>
       </c>
       <c r="H27" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I27" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1677,16 +1689,16 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G28" s="5" t="s">
         <v>30</v>
       </c>
       <c r="H28" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I28" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1697,16 +1709,16 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>29</v>
       </c>
       <c r="H29" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I29" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1717,16 +1729,16 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>31</v>
       </c>
       <c r="H30" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I30" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1737,7 +1749,7 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>32</v>
@@ -1746,7 +1758,7 @@
         <v>32</v>
       </c>
       <c r="I31" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1757,25 +1769,25 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D32" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E32" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="F32" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="H32" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="I32" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1786,22 +1798,22 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
+        <v>195</v>
+      </c>
+      <c r="E33" t="s">
+        <v>109</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H33" t="s">
         <v>202</v>
       </c>
-      <c r="E33" t="s">
-        <v>112</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="H33" t="s">
-        <v>209</v>
-      </c>
       <c r="I33" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1812,25 +1824,25 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D34" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E34" t="s">
         <v>33</v>
       </c>
       <c r="F34" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="G34" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H34" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="I34" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1841,16 +1853,16 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="H35">
         <v>603</v>
       </c>
       <c r="I35" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1861,16 +1873,16 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>34</v>
       </c>
       <c r="H36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I36" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1881,973 +1893,983 @@
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>135</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="H37" t="s">
-        <v>114</v>
+        <v>130</v>
+      </c>
+      <c r="D37" t="s">
+        <v>225</v>
+      </c>
+      <c r="E37" t="s">
+        <v>234</v>
+      </c>
+      <c r="F37" t="s">
+        <v>229</v>
+      </c>
+      <c r="G37" t="s">
+        <v>226</v>
+      </c>
+      <c r="H37">
+        <v>603</v>
       </c>
       <c r="I37" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>136</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H38" t="s">
-        <v>114</v>
+        <v>224</v>
+      </c>
+      <c r="D38" t="s">
+        <v>225</v>
+      </c>
+      <c r="E38" t="s">
+        <v>233</v>
+      </c>
+      <c r="F38" t="s">
+        <v>230</v>
+      </c>
+      <c r="G38" t="s">
+        <v>227</v>
+      </c>
+      <c r="H38">
+        <v>603</v>
       </c>
       <c r="I38" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39">
         <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>137</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H39" t="s">
-        <v>115</v>
+        <v>131</v>
+      </c>
+      <c r="D39" t="s">
+        <v>225</v>
+      </c>
+      <c r="E39" t="s">
+        <v>232</v>
+      </c>
+      <c r="F39" t="s">
+        <v>231</v>
+      </c>
+      <c r="G39" t="s">
+        <v>228</v>
+      </c>
+      <c r="H39">
+        <v>603</v>
       </c>
       <c r="I39" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B40">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>138</v>
+        <v>79</v>
+      </c>
+      <c r="D40" t="s">
+        <v>173</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" t="s">
+        <v>176</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>37</v>
+        <v>174</v>
       </c>
       <c r="H40" t="s">
-        <v>115</v>
+        <v>175</v>
       </c>
       <c r="I40" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>132</v>
       </c>
       <c r="D41" t="s">
-        <v>180</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>38</v>
+        <v>205</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
       </c>
       <c r="F41" t="s">
-        <v>183</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>181</v>
+        <v>207</v>
+      </c>
+      <c r="G41" t="s">
+        <v>204</v>
       </c>
       <c r="H41" t="s">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="I41" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="D42" t="s">
-        <v>212</v>
+        <v>172</v>
       </c>
       <c r="E42" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F42" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G42" t="s">
-        <v>211</v>
+        <v>177</v>
       </c>
       <c r="H42" t="s">
-        <v>213</v>
+        <v>178</v>
       </c>
       <c r="I42" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>83</v>
+        <v>133</v>
       </c>
       <c r="D43" t="s">
-        <v>179</v>
-      </c>
-      <c r="E43" t="s">
-        <v>40</v>
-      </c>
-      <c r="F43" t="s">
-        <v>220</v>
-      </c>
-      <c r="G43" t="s">
-        <v>184</v>
+        <v>170</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="H43" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="I43" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D44" t="s">
-        <v>177</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>41</v>
+        <v>170</v>
+      </c>
+      <c r="E44" t="s">
+        <v>39</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="H44" t="s">
-        <v>216</v>
+        <v>161</v>
       </c>
       <c r="I44" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B45">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>141</v>
-      </c>
-      <c r="D45" t="s">
-        <v>177</v>
-      </c>
-      <c r="E45" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>218</v>
+        <v>40</v>
       </c>
       <c r="H45" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
       <c r="I45" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H46" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I46" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B47">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>142</v>
+        <v>82</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I47" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C48" t="s">
-        <v>85</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>45</v>
+        <v>136</v>
+      </c>
+      <c r="G48" s="5">
+        <v>0</v>
       </c>
       <c r="H48" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="I48" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B49">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>143</v>
-      </c>
-      <c r="G49" s="5">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="H49" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I49" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H50" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I50" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H51" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I51" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H52" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I52" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H53" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I53" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H54" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I54" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H55" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I55" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>146</v>
+        <v>87</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H56" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I56" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C57" t="s">
-        <v>90</v>
+        <v>140</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H57" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I57" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B58">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>147</v>
+        <v>88</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H58" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I58" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>91</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>55</v>
+        <v>141</v>
+      </c>
+      <c r="G59" s="5">
+        <v>51</v>
       </c>
       <c r="H59" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I59" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B60">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>148</v>
-      </c>
-      <c r="G60" s="5">
-        <v>51</v>
+        <v>89</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="H60" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I60" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>92</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>56</v>
+        <v>90</v>
+      </c>
+      <c r="G61" s="5">
+        <v>100</v>
       </c>
       <c r="H61" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I61" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>93</v>
-      </c>
-      <c r="G62" s="5">
-        <v>100</v>
+        <v>91</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="H62" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I62" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H63" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I63" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H64" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I64" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H65" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I65" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H66" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I66" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C67" t="s">
-        <v>98</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>61</v>
+        <v>142</v>
+      </c>
+      <c r="G67" s="5">
+        <v>750</v>
       </c>
       <c r="H67" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I67" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B68">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>149</v>
-      </c>
-      <c r="G68" s="5">
-        <v>750</v>
+        <v>143</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="H68" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I68" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B69">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>150</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>25</v>
+        <v>96</v>
+      </c>
+      <c r="G69" s="5">
+        <v>7.5</v>
       </c>
       <c r="H69" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I69" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B70">
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G70" s="5">
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="H70" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I70" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G71" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H71" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I71" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B72">
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>101</v>
-      </c>
-      <c r="G72" s="5">
-        <v>2</v>
+        <v>99</v>
+      </c>
+      <c r="D72" t="s">
+        <v>219</v>
+      </c>
+      <c r="E72" t="s">
+        <v>216</v>
+      </c>
+      <c r="F72" t="s">
+        <v>221</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>218</v>
       </c>
       <c r="H72" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I72" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B73">
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D73" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="E73" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="F73" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="H73" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I73" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
       <c r="D74" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E74" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
       <c r="F74" t="s">
-        <v>227</v>
-      </c>
-      <c r="G74" s="5" t="s">
-        <v>224</v>
+        <v>192</v>
+      </c>
+      <c r="G74" t="s">
+        <v>196</v>
       </c>
       <c r="H74" t="s">
-        <v>118</v>
+        <v>193</v>
       </c>
       <c r="I74" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="D75" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="E75" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="F75" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G75" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="H75" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="I75" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B76">
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D76" t="s">
-        <v>196</v>
-      </c>
-      <c r="E76" t="s">
-        <v>62</v>
-      </c>
-      <c r="F76" t="s">
-        <v>198</v>
+        <v>158</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="G76" t="s">
-        <v>195</v>
-      </c>
-      <c r="H76" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="I76" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B77">
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D77" t="s">
-        <v>165</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>63</v>
+        <v>180</v>
+      </c>
+      <c r="E77" t="s">
+        <v>181</v>
+      </c>
+      <c r="F77" t="s">
+        <v>214</v>
       </c>
       <c r="G77" t="s">
-        <v>207</v>
+        <v>179</v>
+      </c>
+      <c r="H77" t="s">
+        <v>187</v>
       </c>
       <c r="I77" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
       <c r="D78" t="s">
-        <v>187</v>
+        <v>158</v>
       </c>
       <c r="E78" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F78" t="s">
-        <v>221</v>
+        <v>184</v>
       </c>
       <c r="G78" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H78" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="I78" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B79">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C79" t="s">
-        <v>153</v>
-      </c>
-      <c r="D79" t="s">
-        <v>165</v>
-      </c>
-      <c r="E79" t="s">
-        <v>192</v>
-      </c>
-      <c r="F79" t="s">
-        <v>191</v>
-      </c>
-      <c r="G79" t="s">
-        <v>189</v>
+        <v>145</v>
+      </c>
+      <c r="G79" s="5" t="s">
+        <v>164</v>
       </c>
       <c r="H79" t="s">
-        <v>190</v>
+        <v>61</v>
       </c>
       <c r="I79" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>78</v>
-      </c>
-      <c r="B80">
-        <v>40</v>
-      </c>
-      <c r="C80" t="s">
-        <v>152</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="H80" t="s">
-        <v>64</v>
-      </c>
-      <c r="I80" t="s">
-        <v>124</v>
-      </c>
+      <c r="G80" s="5"/>
     </row>
     <row r="81" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G81" s="5"/>
@@ -2884,9 +2906,6 @@
     </row>
     <row r="92" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G92" s="5"/>
-    </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G93" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated test points on bom
</commit_message>
<xml_diff>
--- a/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
+++ b/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="237">
   <si>
     <t>Item #</t>
   </si>
@@ -510,9 +510,6 @@
     <t>Header</t>
   </si>
   <si>
-    <t>Testpoint</t>
-  </si>
-  <si>
     <t xml:space="preserve">MOSFET 50V 200mW </t>
   </si>
   <si>
@@ -721,6 +718,15 @@
   </si>
   <si>
     <t>APT1608SYCK</t>
+  </si>
+  <si>
+    <t>Keystone Electronics</t>
+  </si>
+  <si>
+    <t>5006K-ND</t>
+  </si>
+  <si>
+    <t>TEST POINT PC COMPACT .063"D BLK</t>
   </si>
 </sst>
 </file>
@@ -1092,9 +1098,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1173,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>148</v>
@@ -1187,7 +1193,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>149</v>
@@ -1230,7 +1236,7 @@
         <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E7" t="s">
         <v>151</v>
@@ -1308,7 +1314,7 @@
         <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -1337,10 +1343,10 @@
         <v>158</v>
       </c>
       <c r="E11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G11" t="s">
         <v>160</v>
@@ -1363,16 +1369,16 @@
         <v>66</v>
       </c>
       <c r="D12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
@@ -1772,19 +1778,19 @@
         <v>129</v>
       </c>
       <c r="D32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E32" t="s">
+        <v>167</v>
+      </c>
+      <c r="F32" t="s">
+        <v>211</v>
+      </c>
+      <c r="G32" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="F32" t="s">
-        <v>212</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>169</v>
-      </c>
       <c r="H32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I32" t="s">
         <v>119</v>
@@ -1801,16 +1807,16 @@
         <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E33" t="s">
         <v>109</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="I33" t="s">
         <v>119</v>
@@ -1827,19 +1833,19 @@
         <v>76</v>
       </c>
       <c r="D34" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E34" t="s">
         <v>33</v>
       </c>
       <c r="F34" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G34" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I34" t="s">
         <v>119</v>
@@ -1856,7 +1862,7 @@
         <v>77</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H35">
         <v>603</v>
@@ -1896,16 +1902,16 @@
         <v>130</v>
       </c>
       <c r="D37" t="s">
+        <v>224</v>
+      </c>
+      <c r="E37" t="s">
+        <v>233</v>
+      </c>
+      <c r="F37" t="s">
+        <v>228</v>
+      </c>
+      <c r="G37" t="s">
         <v>225</v>
-      </c>
-      <c r="E37" t="s">
-        <v>234</v>
-      </c>
-      <c r="F37" t="s">
-        <v>229</v>
-      </c>
-      <c r="G37" t="s">
-        <v>226</v>
       </c>
       <c r="H37">
         <v>603</v>
@@ -1922,19 +1928,19 @@
         <v>9</v>
       </c>
       <c r="C38" t="s">
+        <v>223</v>
+      </c>
+      <c r="D38" t="s">
         <v>224</v>
       </c>
-      <c r="D38" t="s">
-        <v>225</v>
-      </c>
       <c r="E38" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F38" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H38">
         <v>603</v>
@@ -1954,16 +1960,16 @@
         <v>131</v>
       </c>
       <c r="D39" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G39" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H39">
         <v>603</v>
@@ -1983,19 +1989,19 @@
         <v>79</v>
       </c>
       <c r="D40" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>35</v>
       </c>
       <c r="F40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G40" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H40" t="s">
         <v>174</v>
-      </c>
-      <c r="H40" t="s">
-        <v>175</v>
       </c>
       <c r="I40" t="s">
         <v>119</v>
@@ -2012,19 +2018,19 @@
         <v>132</v>
       </c>
       <c r="D41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E41" t="s">
         <v>36</v>
       </c>
       <c r="F41" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I41" t="s">
         <v>119</v>
@@ -2041,19 +2047,19 @@
         <v>80</v>
       </c>
       <c r="D42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E42" t="s">
         <v>37</v>
       </c>
       <c r="F42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G42" t="s">
+        <v>176</v>
+      </c>
+      <c r="H42" t="s">
         <v>177</v>
-      </c>
-      <c r="H42" t="s">
-        <v>178</v>
       </c>
       <c r="I42" t="s">
         <v>119</v>
@@ -2070,16 +2076,16 @@
         <v>133</v>
       </c>
       <c r="D43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>38</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H43" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I43" t="s">
         <v>119</v>
@@ -2096,13 +2102,13 @@
         <v>134</v>
       </c>
       <c r="D44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E44" t="s">
         <v>39</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H44" t="s">
         <v>161</v>
@@ -2662,16 +2668,16 @@
         <v>99</v>
       </c>
       <c r="D72" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E72" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F72" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H72" t="s">
         <v>113</v>
@@ -2691,16 +2697,16 @@
         <v>100</v>
       </c>
       <c r="D73" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E73" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F73" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H73" t="s">
         <v>113</v>
@@ -2720,19 +2726,19 @@
         <v>144</v>
       </c>
       <c r="D74" t="s">
+        <v>194</v>
+      </c>
+      <c r="E74" t="s">
+        <v>193</v>
+      </c>
+      <c r="F74" t="s">
+        <v>191</v>
+      </c>
+      <c r="G74" t="s">
         <v>195</v>
       </c>
-      <c r="E74" t="s">
-        <v>194</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="H74" t="s">
         <v>192</v>
-      </c>
-      <c r="G74" t="s">
-        <v>196</v>
-      </c>
-      <c r="H74" t="s">
-        <v>193</v>
       </c>
       <c r="I74" t="s">
         <v>119</v>
@@ -2749,19 +2755,19 @@
         <v>101</v>
       </c>
       <c r="D75" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E75" t="s">
         <v>59</v>
       </c>
       <c r="F75" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G75" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H75" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I75" t="s">
         <v>119</v>
@@ -2784,7 +2790,7 @@
         <v>60</v>
       </c>
       <c r="G76" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I76" t="s">
         <v>119</v>
@@ -2801,19 +2807,19 @@
         <v>103</v>
       </c>
       <c r="D77" t="s">
+        <v>179</v>
+      </c>
+      <c r="E77" t="s">
         <v>180</v>
       </c>
-      <c r="E77" t="s">
-        <v>181</v>
-      </c>
       <c r="F77" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G77" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H77" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I77" t="s">
         <v>119</v>
@@ -2833,16 +2839,16 @@
         <v>158</v>
       </c>
       <c r="E78" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F78" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G78" t="s">
+        <v>181</v>
+      </c>
+      <c r="H78" t="s">
         <v>182</v>
-      </c>
-      <c r="H78" t="s">
-        <v>183</v>
       </c>
       <c r="I78" t="s">
         <v>119</v>
@@ -2858,8 +2864,17 @@
       <c r="C79" t="s">
         <v>145</v>
       </c>
+      <c r="D79" t="s">
+        <v>234</v>
+      </c>
+      <c r="E79">
+        <v>5006</v>
+      </c>
+      <c r="F79" t="s">
+        <v>235</v>
+      </c>
       <c r="G79" s="5" t="s">
-        <v>164</v>
+        <v>236</v>
       </c>
       <c r="H79" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
Replaced 2 ohm resistor; updated bom
</commit_message>
<xml_diff>
--- a/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
+++ b/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="10035"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="244">
   <si>
     <t>Item #</t>
   </si>
@@ -733,6 +733,21 @@
   </si>
   <si>
     <t>154k, Resistor, Chip, 1/16W, 1%</t>
+  </si>
+  <si>
+    <t>RMCF2512FT2R00CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF2512FT2R00</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t>RES 2 OHM 1W 1%</t>
+  </si>
+  <si>
+    <t>2512</t>
   </si>
 </sst>
 </file>
@@ -1106,9 +1121,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3008,19 +3023,19 @@
         <v>71</v>
       </c>
       <c r="D70" t="s">
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="E70" t="s">
-        <v>201</v>
+        <v>240</v>
       </c>
       <c r="F70" t="s">
-        <v>201</v>
-      </c>
-      <c r="G70" s="5">
-        <v>2</v>
+        <v>239</v>
+      </c>
+      <c r="G70" t="s">
+        <v>242</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>205</v>
+        <v>243</v>
       </c>
       <c r="I70" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Added D1,D2,D3 part number in schematic and bom
</commit_message>
<xml_diff>
--- a/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
+++ b/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="251">
   <si>
     <t>Item #</t>
   </si>
@@ -66,9 +66,6 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>DIODE-0603</t>
-  </si>
-  <si>
     <t>KS8999</t>
   </si>
   <si>
@@ -297,9 +294,6 @@
     <t>C117,C118,C119,C120.C123,C125</t>
   </si>
   <si>
-    <t>D1,D2,D3</t>
-  </si>
-  <si>
     <t>Q2,Q3,Q4</t>
   </si>
   <si>
@@ -748,6 +742,33 @@
   </si>
   <si>
     <t>2512</t>
+  </si>
+  <si>
+    <t>D2,D3</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Comchip Technology</t>
+  </si>
+  <si>
+    <t>CDBU0520</t>
+  </si>
+  <si>
+    <t>641-1332-1-ND</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 0.5A</t>
+  </si>
+  <si>
+    <t>641-1282-1-ND</t>
+  </si>
+  <si>
+    <t>CDBU0130L</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 30V 0.1A</t>
   </si>
 </sst>
 </file>
@@ -1119,11 +1140,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,13 +1200,13 @@
         <v>9</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1196,16 +1217,16 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1216,16 +1237,16 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1236,16 +1257,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1256,22 +1277,22 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1282,22 +1303,22 @@
         <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1308,22 +1329,22 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" t="s">
         <v>117</v>
       </c>
-      <c r="E9" t="s">
-        <v>119</v>
-      </c>
       <c r="G9" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H9" t="s">
         <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1334,22 +1355,22 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1360,25 +1381,25 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" t="s">
         <v>122</v>
       </c>
-      <c r="E11" t="s">
-        <v>130</v>
-      </c>
-      <c r="F11" t="s">
-        <v>161</v>
-      </c>
-      <c r="G11" t="s">
-        <v>124</v>
-      </c>
       <c r="H11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1389,25 +1410,25 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1418,25 +1439,25 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1447,25 +1468,25 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1476,25 +1497,25 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1505,25 +1526,25 @@
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1534,25 +1555,25 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1563,25 +1584,25 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1592,25 +1613,25 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1621,25 +1642,25 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1650,25 +1671,25 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F21" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1679,25 +1700,25 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1708,25 +1729,25 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F23" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1737,25 +1758,25 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
+        <v>199</v>
+      </c>
+      <c r="E24" t="s">
+        <v>199</v>
+      </c>
+      <c r="F24" t="s">
+        <v>199</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H24" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="E24" t="s">
-        <v>201</v>
-      </c>
-      <c r="F24" t="s">
-        <v>201</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>203</v>
-      </c>
       <c r="I24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1766,25 +1787,25 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
+        <v>199</v>
+      </c>
+      <c r="E25" t="s">
+        <v>199</v>
+      </c>
+      <c r="F25" t="s">
+        <v>199</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="E25" t="s">
-        <v>201</v>
-      </c>
-      <c r="F25" t="s">
-        <v>201</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>203</v>
-      </c>
       <c r="I25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1795,25 +1816,25 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
+        <v>199</v>
+      </c>
+      <c r="E26" t="s">
+        <v>199</v>
+      </c>
+      <c r="F26" t="s">
+        <v>199</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="E26" t="s">
-        <v>201</v>
-      </c>
-      <c r="F26" t="s">
-        <v>201</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>203</v>
-      </c>
       <c r="I26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1824,25 +1845,25 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D27" t="s">
+        <v>199</v>
+      </c>
+      <c r="E27" t="s">
+        <v>199</v>
+      </c>
+      <c r="F27" t="s">
+        <v>199</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="E27" t="s">
-        <v>201</v>
-      </c>
-      <c r="F27" t="s">
-        <v>201</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>203</v>
-      </c>
       <c r="I27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1853,25 +1874,25 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E28" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F28" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1882,25 +1903,25 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1911,25 +1932,25 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F30" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1937,1338 +1958,1373 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" t="s">
-        <v>16</v>
+        <v>243</v>
+      </c>
+      <c r="D31" t="s">
+        <v>244</v>
+      </c>
+      <c r="E31" t="s">
+        <v>245</v>
+      </c>
+      <c r="F31" t="s">
+        <v>246</v>
+      </c>
+      <c r="G31" t="s">
+        <v>247</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="I31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>242</v>
       </c>
       <c r="D32" t="s">
-        <v>133</v>
+        <v>244</v>
       </c>
       <c r="E32" t="s">
-        <v>131</v>
-      </c>
-      <c r="F32" t="s">
-        <v>175</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H32" t="s">
-        <v>141</v>
+        <v>249</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="G32" t="s">
+        <v>250</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="I32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="D33" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="E33" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="F33" t="s">
-        <v>226</v>
+        <v>173</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H33" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="I33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D34" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="E34" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="F34" t="s">
-        <v>162</v>
-      </c>
-      <c r="G34" t="s">
-        <v>171</v>
+        <v>224</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="H34" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="I34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>203</v>
+        <v>49</v>
+      </c>
+      <c r="D35" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" t="s">
+        <v>160</v>
+      </c>
+      <c r="G35" t="s">
+        <v>169</v>
+      </c>
+      <c r="H35" t="s">
+        <v>147</v>
       </c>
       <c r="I35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" t="s">
-        <v>223</v>
-      </c>
-      <c r="E36" t="s">
-        <v>224</v>
-      </c>
-      <c r="F36" t="s">
-        <v>225</v>
+        <v>50</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="H36" t="s">
-        <v>78</v>
+        <v>164</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="I36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="D37" t="s">
-        <v>188</v>
+        <v>221</v>
       </c>
       <c r="E37" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
       <c r="F37" t="s">
-        <v>192</v>
-      </c>
-      <c r="G37" t="s">
-        <v>189</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>203</v>
+        <v>223</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="H37" t="s">
+        <v>77</v>
       </c>
       <c r="I37" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38">
         <v>9</v>
       </c>
       <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
+        <v>186</v>
+      </c>
+      <c r="E38" t="s">
+        <v>195</v>
+      </c>
+      <c r="F38" t="s">
+        <v>190</v>
+      </c>
+      <c r="G38" t="s">
         <v>187</v>
       </c>
-      <c r="D38" t="s">
-        <v>188</v>
-      </c>
-      <c r="E38" t="s">
-        <v>196</v>
-      </c>
-      <c r="F38" t="s">
-        <v>193</v>
-      </c>
-      <c r="G38" t="s">
-        <v>190</v>
-      </c>
       <c r="H38" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>185</v>
       </c>
       <c r="D39" t="s">
+        <v>186</v>
+      </c>
+      <c r="E39" t="s">
+        <v>194</v>
+      </c>
+      <c r="F39" t="s">
+        <v>191</v>
+      </c>
+      <c r="G39" t="s">
         <v>188</v>
       </c>
-      <c r="E39" t="s">
-        <v>195</v>
-      </c>
-      <c r="F39" t="s">
-        <v>194</v>
-      </c>
-      <c r="G39" t="s">
-        <v>191</v>
-      </c>
       <c r="H39" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I39" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>18</v>
+        <v>186</v>
+      </c>
+      <c r="E40" t="s">
+        <v>193</v>
       </c>
       <c r="F40" t="s">
-        <v>139</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="H40" t="s">
-        <v>138</v>
+        <v>192</v>
+      </c>
+      <c r="G40" t="s">
+        <v>189</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="I40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="D41" t="s">
-        <v>168</v>
-      </c>
-      <c r="E41" t="s">
-        <v>19</v>
+        <v>134</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="F41" t="s">
-        <v>170</v>
-      </c>
-      <c r="G41" t="s">
-        <v>167</v>
+        <v>137</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>135</v>
       </c>
       <c r="H41" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="I41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>54</v>
+        <v>95</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>166</v>
       </c>
       <c r="E42" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F42" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G42" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="H42" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="I42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="D43" t="s">
         <v>133</v>
       </c>
-      <c r="E43" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>173</v>
+      <c r="E43" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" t="s">
+        <v>174</v>
+      </c>
+      <c r="G43" t="s">
+        <v>138</v>
       </c>
       <c r="H43" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="I43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D44" t="s">
-        <v>133</v>
-      </c>
-      <c r="E44" t="s">
-        <v>22</v>
+        <v>131</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H44" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
       <c r="I44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>55</v>
+        <v>97</v>
+      </c>
+      <c r="D45" t="s">
+        <v>131</v>
+      </c>
+      <c r="E45" t="s">
+        <v>21</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>23</v>
+        <v>172</v>
       </c>
       <c r="H45" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="I45" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H46" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>56</v>
+        <v>98</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H47" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I47" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
-      </c>
-      <c r="D48" t="s">
-        <v>201</v>
-      </c>
-      <c r="E48" t="s">
-        <v>201</v>
-      </c>
-      <c r="F48" t="s">
-        <v>201</v>
+        <v>55</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>202</v>
+        <v>24</v>
+      </c>
+      <c r="H48" t="s">
+        <v>24</v>
       </c>
       <c r="I48" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="D49" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E49" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F49" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>26</v>
+        <v>225</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D50" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E50" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F50" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>230</v>
+        <v>25</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="D51" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E51" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F51" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>27</v>
+        <v>228</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D52" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E52" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F52" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="D53" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E53" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F53" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D54" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E54" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F54" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="D55" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E55" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F55" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>229</v>
+        <v>29</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>235</v>
+        <v>102</v>
       </c>
       <c r="D56" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E56" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F56" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>233</v>
       </c>
       <c r="D57" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E57" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F57" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="D58" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E58" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F58" t="s">
-        <v>201</v>
-      </c>
-      <c r="G58" s="5">
-        <v>51</v>
+        <v>199</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I58" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="D59" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E59" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F59" t="s">
-        <v>201</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>231</v>
+        <v>199</v>
+      </c>
+      <c r="G59" s="5">
+        <v>51</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D60" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E60" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F60" t="s">
-        <v>201</v>
-      </c>
-      <c r="G60" s="5">
-        <v>100</v>
+        <v>199</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>229</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D61" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E61" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F61" t="s">
-        <v>201</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>32</v>
+        <v>199</v>
+      </c>
+      <c r="G61" s="5">
+        <v>100</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D62" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E62" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F62" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>236</v>
+        <v>31</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D63" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E63" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F63" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I63" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D64" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E64" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F64" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I64" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D65" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E65" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F65" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I65" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="D66" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E66" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F66" t="s">
-        <v>201</v>
-      </c>
-      <c r="G66" s="5">
-        <v>750</v>
+        <v>199</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>230</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C67" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D67" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E67" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F67" t="s">
-        <v>201</v>
-      </c>
-      <c r="G67" s="5" t="s">
-        <v>15</v>
+        <v>199</v>
+      </c>
+      <c r="G67" s="5">
+        <v>750</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I67" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>69</v>
+        <v>105</v>
       </c>
       <c r="D68" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E68" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F68" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="H68" s="6" t="s">
-        <v>203</v>
+        <v>15</v>
+      </c>
+      <c r="H68" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="I68" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69">
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D69" t="s">
+        <v>199</v>
+      </c>
+      <c r="E69" t="s">
+        <v>199</v>
+      </c>
+      <c r="F69" t="s">
+        <v>199</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="H69" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="E69" t="s">
-        <v>201</v>
-      </c>
-      <c r="F69" t="s">
-        <v>201</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>203</v>
-      </c>
       <c r="I69" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70">
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D70" t="s">
-        <v>241</v>
+        <v>199</v>
       </c>
       <c r="E70" t="s">
-        <v>240</v>
+        <v>199</v>
       </c>
       <c r="F70" t="s">
-        <v>239</v>
-      </c>
-      <c r="G70" t="s">
-        <v>242</v>
+        <v>199</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>231</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>243</v>
+        <v>201</v>
       </c>
       <c r="I70" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>182</v>
+        <v>239</v>
       </c>
       <c r="E71" t="s">
-        <v>179</v>
+        <v>238</v>
       </c>
       <c r="F71" t="s">
-        <v>184</v>
-      </c>
-      <c r="G71" s="5" t="s">
-        <v>181</v>
+        <v>237</v>
+      </c>
+      <c r="G71" t="s">
+        <v>240</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>205</v>
+        <v>241</v>
       </c>
       <c r="I71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72">
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D72" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="E72" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I72" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="D73" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E73" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="F73" t="s">
-        <v>155</v>
-      </c>
-      <c r="G73" t="s">
-        <v>159</v>
-      </c>
-      <c r="H73" t="s">
-        <v>156</v>
+        <v>181</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>203</v>
       </c>
       <c r="I73" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="D74" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E74" t="s">
-        <v>33</v>
+        <v>155</v>
       </c>
       <c r="F74" t="s">
+        <v>153</v>
+      </c>
+      <c r="G74" t="s">
+        <v>157</v>
+      </c>
+      <c r="H74" t="s">
         <v>154</v>
       </c>
-      <c r="G74" t="s">
-        <v>151</v>
-      </c>
-      <c r="H74" t="s">
-        <v>153</v>
-      </c>
       <c r="I74" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
+        <v>72</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
         <v>73</v>
       </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
-      <c r="C75" t="s">
-        <v>75</v>
-      </c>
       <c r="D75" t="s">
-        <v>122</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>34</v>
+        <v>150</v>
+      </c>
+      <c r="E75" t="s">
+        <v>32</v>
+      </c>
+      <c r="F75" t="s">
+        <v>152</v>
       </c>
       <c r="G75" t="s">
-        <v>163</v>
+        <v>149</v>
+      </c>
+      <c r="H75" t="s">
+        <v>151</v>
       </c>
       <c r="I75" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
+        <v>73</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
         <v>74</v>
       </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-      <c r="C76" t="s">
-        <v>76</v>
-      </c>
       <c r="D76" t="s">
-        <v>143</v>
-      </c>
-      <c r="E76" t="s">
-        <v>144</v>
-      </c>
-      <c r="F76" t="s">
-        <v>177</v>
+        <v>120</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="G76" t="s">
-        <v>142</v>
-      </c>
-      <c r="H76" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="I76" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
+        <v>74</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
         <v>75</v>
       </c>
-      <c r="B77">
-        <v>7</v>
-      </c>
-      <c r="C77" t="s">
-        <v>110</v>
-      </c>
       <c r="D77" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
       <c r="E77" t="s">
+        <v>142</v>
+      </c>
+      <c r="F77" t="s">
+        <v>175</v>
+      </c>
+      <c r="G77" t="s">
+        <v>140</v>
+      </c>
+      <c r="H77" t="s">
         <v>148</v>
       </c>
-      <c r="F77" t="s">
-        <v>147</v>
-      </c>
-      <c r="G77" t="s">
-        <v>145</v>
-      </c>
-      <c r="H77" t="s">
-        <v>146</v>
-      </c>
       <c r="I77" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
+        <v>75</v>
+      </c>
+      <c r="B78">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>108</v>
+      </c>
+      <c r="D78" t="s">
+        <v>120</v>
+      </c>
+      <c r="E78" t="s">
+        <v>146</v>
+      </c>
+      <c r="F78" t="s">
+        <v>145</v>
+      </c>
+      <c r="G78" t="s">
+        <v>143</v>
+      </c>
+      <c r="H78" t="s">
+        <v>144</v>
+      </c>
+      <c r="I78" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>76</v>
       </c>
-      <c r="B78">
+      <c r="B79">
         <v>40</v>
       </c>
-      <c r="C78" t="s">
-        <v>109</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="C79" t="s">
+        <v>107</v>
+      </c>
+      <c r="D79" t="s">
+        <v>196</v>
+      </c>
+      <c r="E79">
+        <v>5006</v>
+      </c>
+      <c r="F79" t="s">
+        <v>197</v>
+      </c>
+      <c r="G79" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="E78">
-        <v>5006</v>
-      </c>
-      <c r="F78" t="s">
-        <v>199</v>
-      </c>
-      <c r="G78" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="H78" t="s">
-        <v>35</v>
-      </c>
-      <c r="I78" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G79" s="5"/>
+      <c r="H79" t="s">
+        <v>34</v>
+      </c>
+      <c r="I79" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G80" s="5"/>
@@ -3305,6 +3361,9 @@
     </row>
     <row r="91" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G91" s="5"/>
+    </row>
+    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G92" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added header parts for bom
</commit_message>
<xml_diff>
--- a/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
+++ b/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="253">
   <si>
     <t>Item #</t>
   </si>
@@ -120,9 +120,6 @@
     <t>SN65220DBV</t>
   </si>
   <si>
-    <t>TPTP06R</t>
-  </si>
-  <si>
     <t>J22</t>
   </si>
   <si>
@@ -339,21 +336,9 @@
     <t>Q5,Q7</t>
   </si>
   <si>
-    <t>TP1,TP2,TP3,TP4,TP5,TP6,TP7,TP8,TP9,TP10,TP11,TP12,TP13,TP14,TP15,TP16,TP17,TP18,TP19,TP20,TP21,TP22,TP23,TP24,TP25,TP26,TP27,TP28,TP29,TP30,TP31,TP32,TP33,TP34,TP35,TP36,TP37,TP38,TP39,TP40</t>
-  </si>
-  <si>
     <t>U7,U8,U9,U10,U11,U12,U13</t>
   </si>
   <si>
-    <t>50 mil (1.27 mm) Inline 1x3 Male Header</t>
-  </si>
-  <si>
-    <t>50 mil (1.27 mm) Inline 1x4 Male Header</t>
-  </si>
-  <si>
-    <t>50 mil (1.27 mm) Inline 1x2 Male Header</t>
-  </si>
-  <si>
     <t>50 mil (1.27 mm)  2x5 Male Header</t>
   </si>
   <si>
@@ -606,15 +591,6 @@
     <t>APT1608SYCK</t>
   </si>
   <si>
-    <t>Keystone Electronics</t>
-  </si>
-  <si>
-    <t>5006K-ND</t>
-  </si>
-  <si>
-    <t>TEST POINT PC COMPACT .063"D BLK</t>
-  </si>
-  <si>
     <t>Std</t>
   </si>
   <si>
@@ -769,6 +745,36 @@
   </si>
   <si>
     <t>DIODE SCHOTTKY 30V 0.1A</t>
+  </si>
+  <si>
+    <t>S9014E-02-ND</t>
+  </si>
+  <si>
+    <t>GRPB021VWVN-RC</t>
+  </si>
+  <si>
+    <t>Sullins Connector Solutions</t>
+  </si>
+  <si>
+    <t>CONN HEADER .050" 2POS PCB GOLD</t>
+  </si>
+  <si>
+    <t>S9014E-03-ND</t>
+  </si>
+  <si>
+    <t>GRPB031VWVN-RC</t>
+  </si>
+  <si>
+    <t>CONN HEADER .050" 3POS PCB GOLD</t>
+  </si>
+  <si>
+    <t>S9014E-04-ND</t>
+  </si>
+  <si>
+    <t>GRPB041VWVN-RC</t>
+  </si>
+  <si>
+    <t>CONN HEADER .050" 4POS PCB GOLD</t>
   </si>
 </sst>
 </file>
@@ -1143,8 +1149,8 @@
   <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1199,14 +1205,23 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>109</v>
+      <c r="D3" t="s">
+        <v>245</v>
+      </c>
+      <c r="E3" t="s">
+        <v>248</v>
+      </c>
+      <c r="F3" t="s">
+        <v>247</v>
+      </c>
+      <c r="G3" t="s">
+        <v>249</v>
       </c>
       <c r="H3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1217,19 +1232,28 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>110</v>
+        <v>179</v>
+      </c>
+      <c r="D4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F4" t="s">
+        <v>250</v>
+      </c>
+      <c r="G4" t="s">
+        <v>252</v>
       </c>
       <c r="H4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1237,19 +1261,28 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>183</v>
+        <v>178</v>
+      </c>
+      <c r="D5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E5" t="s">
+        <v>244</v>
+      </c>
+      <c r="F5" t="s">
+        <v>243</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>111</v>
+        <v>246</v>
       </c>
       <c r="H5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1257,16 +1290,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="H6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1277,22 +1310,22 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1303,22 +1336,22 @@
         <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1329,22 +1362,22 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E9" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="H9" t="s">
         <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1355,22 +1388,22 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H10" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1381,25 +1414,25 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F11" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="H11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1410,25 +1443,25 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1439,25 +1472,25 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E13" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F13" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1468,25 +1501,25 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E14" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F14" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1497,25 +1530,25 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E15" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F15" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1526,25 +1559,25 @@
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E16" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F16" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1555,25 +1588,25 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
+        <v>191</v>
+      </c>
+      <c r="E17" t="s">
+        <v>191</v>
+      </c>
+      <c r="F17" t="s">
+        <v>191</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="E17" t="s">
-        <v>199</v>
-      </c>
-      <c r="F17" t="s">
-        <v>199</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>207</v>
-      </c>
       <c r="H17" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1584,25 +1617,25 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E18" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F18" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1613,25 +1646,25 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E19" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F19" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1642,25 +1675,25 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F20" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1671,25 +1704,25 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E21" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F21" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1700,25 +1733,25 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E22" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F22" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1729,25 +1762,25 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E23" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F23" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1758,25 +1791,25 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D24" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E24" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F24" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1787,25 +1820,25 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D25" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E25" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F25" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1816,25 +1849,25 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E26" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F26" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1845,25 +1878,25 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E27" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F27" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1874,25 +1907,25 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E28" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F28" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="I28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1903,25 +1936,25 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E29" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F29" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="I29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1932,25 +1965,25 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E30" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F30" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="I30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1961,427 +1994,427 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D31" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="E31" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="F31" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="G31" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" t="s">
+        <v>234</v>
+      </c>
+      <c r="D32" t="s">
+        <v>236</v>
+      </c>
+      <c r="E32" t="s">
+        <v>241</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="G32" t="s">
         <v>242</v>
       </c>
-      <c r="D32" t="s">
-        <v>244</v>
-      </c>
-      <c r="E32" t="s">
-        <v>249</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="G32" t="s">
-        <v>250</v>
-      </c>
       <c r="H32" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E33" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F33" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H33" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="I33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F34" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H34" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="I34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D35" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E35" t="s">
         <v>16</v>
       </c>
       <c r="F35" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G35" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H35" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="I35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="E37" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F37" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="H37" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E38" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F38" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G38" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D39" t="s">
+        <v>181</v>
+      </c>
+      <c r="E39" t="s">
+        <v>189</v>
+      </c>
+      <c r="F39" t="s">
         <v>186</v>
       </c>
-      <c r="E39" t="s">
-        <v>194</v>
-      </c>
-      <c r="F39" t="s">
-        <v>191</v>
-      </c>
       <c r="G39" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E40" t="s">
+        <v>188</v>
+      </c>
+      <c r="F40" t="s">
+        <v>187</v>
+      </c>
+      <c r="G40" t="s">
+        <v>184</v>
+      </c>
+      <c r="H40" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="F40" t="s">
-        <v>192</v>
-      </c>
-      <c r="G40" t="s">
-        <v>189</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>201</v>
-      </c>
       <c r="I40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D41" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F41" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H41" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D42" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E42" t="s">
         <v>18</v>
       </c>
       <c r="F42" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G42" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H42" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D43" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E43" t="s">
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="G43" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H43" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="I43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>20</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H44" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="I44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D45" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E45" t="s">
         <v>21</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H45" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>22</v>
@@ -2390,18 +2423,18 @@
         <v>22</v>
       </c>
       <c r="I46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>23</v>
@@ -2410,18 +2443,18 @@
         <v>23</v>
       </c>
       <c r="I47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>24</v>
@@ -2430,901 +2463,875 @@
         <v>24</v>
       </c>
       <c r="I48" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D49" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E49" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F49" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D50" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E50" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F50" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D51" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E51" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F51" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D52" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E52" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F52" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D53" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E53" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F53" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D54" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E54" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F54" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>28</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D55" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E55" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F55" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>29</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D56" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E56" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F56" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>25</v>
       </c>
       <c r="C57" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D57" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E57" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F57" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I57" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D58" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E58" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F58" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>30</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D59" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E59" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F59" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G59" s="5">
         <v>51</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D60" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E60" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F60" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D61" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E61" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F61" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G61" s="5">
         <v>100</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D62" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E62" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F62" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>31</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D63" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E63" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F63" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D64" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E64" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F64" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D65" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E65" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F65" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I65" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D66" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E66" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F66" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I66" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B67">
         <v>27</v>
       </c>
       <c r="C67" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D67" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E67" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F67" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G67" s="5">
         <v>750</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B68">
         <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D68" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E68" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F68" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="I68" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B69">
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D69" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E69" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F69" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B70">
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D70" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E70" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="F70" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I70" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B71">
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D71" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="E71" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="F71" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="G71" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="I71" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B72">
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D72" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E72" t="s">
+        <v>172</v>
+      </c>
+      <c r="F72" t="s">
         <v>177</v>
       </c>
-      <c r="F72" t="s">
-        <v>182</v>
-      </c>
       <c r="G72" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="I72" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B73">
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D73" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E73" t="s">
+        <v>171</v>
+      </c>
+      <c r="F73" t="s">
         <v>176</v>
       </c>
-      <c r="F73" t="s">
-        <v>181</v>
-      </c>
       <c r="G73" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="I73" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B74">
         <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D74" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E74" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F74" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="G74" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H74" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="I74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
         <v>72</v>
       </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
-      <c r="C75" t="s">
-        <v>73</v>
-      </c>
       <c r="D75" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E75" t="s">
         <v>32</v>
       </c>
       <c r="F75" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G75" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="H75" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
         <v>73</v>
       </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-      <c r="C76" t="s">
-        <v>74</v>
-      </c>
       <c r="D76" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>33</v>
       </c>
       <c r="G76" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="I76" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
         <v>74</v>
       </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
-      <c r="C77" t="s">
-        <v>75</v>
-      </c>
       <c r="D77" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E77" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F77" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G77" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H77" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="I77" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B78">
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D78" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E78" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F78" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G78" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H78" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I78" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>76</v>
-      </c>
-      <c r="B79">
-        <v>40</v>
-      </c>
-      <c r="C79" t="s">
-        <v>107</v>
-      </c>
-      <c r="D79" t="s">
-        <v>196</v>
-      </c>
-      <c r="E79">
-        <v>5006</v>
-      </c>
-      <c r="F79" t="s">
-        <v>197</v>
-      </c>
-      <c r="G79" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="H79" t="s">
-        <v>34</v>
-      </c>
-      <c r="I79" t="s">
-        <v>83</v>
-      </c>
+      <c r="G79" s="5"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G80" s="5"/>

</xml_diff>

<commit_message>
Added ferrite bead part to bom
</commit_message>
<xml_diff>
--- a/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
+++ b/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="258">
   <si>
     <t>Item #</t>
   </si>
@@ -339,9 +339,6 @@
     <t>U7,U8,U9,U10,U11,U12,U13</t>
   </si>
   <si>
-    <t>50 mil (1.27 mm)  2x5 Male Header</t>
-  </si>
-  <si>
     <t>8Y-25.000MEEQ-T</t>
   </si>
   <si>
@@ -495,9 +492,6 @@
     <t>Non-Standard (Custom size)</t>
   </si>
   <si>
-    <t>Ferrite Bead</t>
-  </si>
-  <si>
     <t>0.8 Ohm, Low-Voltage, 4-Channel Analog Multiplexer</t>
   </si>
   <si>
@@ -606,36 +600,9 @@
     <t>1206</t>
   </si>
   <si>
-    <t>1n, Capacitor, Ceramic,  X7R, 10%</t>
-  </si>
-  <si>
-    <t>0.047uF, Capacitor, Ceramic,  X7R, 10%</t>
-  </si>
-  <si>
-    <t>0.01uF, Capacitor, Ceramic,  X7R, 10%</t>
-  </si>
-  <si>
     <t>2.2u/Low ESR, Capacitor, Ceramic,  X7R, 10%</t>
   </si>
   <si>
-    <t>10nF, Capacitor, Ceramic,  X7R, 10%</t>
-  </si>
-  <si>
-    <t>10p, Capacitor, Ceramic,  X7R, 10%</t>
-  </si>
-  <si>
-    <t>100n/40V, Capacitor, Ceramic,  X7R, 10%</t>
-  </si>
-  <si>
-    <t>0.1uF/40V, Capacitor, Ceramic,  X7R, 10%</t>
-  </si>
-  <si>
-    <t>100pF, Capacitor, Ceramic,  X7R, 10%</t>
-  </si>
-  <si>
-    <t>2200pF/40V, Capacitor, Ceramic,  X7R, 10%</t>
-  </si>
-  <si>
     <t>10uF, Capacitor, Ceramic,  X7R, 10%</t>
   </si>
   <si>
@@ -775,6 +742,54 @@
   </si>
   <si>
     <t>CONN HEADER .050" 4POS PCB GOLD</t>
+  </si>
+  <si>
+    <t>GRPB052VWVN-RC</t>
+  </si>
+  <si>
+    <t>S9015E-05-ND</t>
+  </si>
+  <si>
+    <t>CONN HEADER .050" 10PS DL PCB AU</t>
+  </si>
+  <si>
+    <t>10p, Capacitor, Ceramic,  C0G, 1%</t>
+  </si>
+  <si>
+    <t>100pF, Capacitor, Ceramic,  X7R, 5%</t>
+  </si>
+  <si>
+    <t>2200pF/40V, Capacitor, Ceramic,  X7R, 5%</t>
+  </si>
+  <si>
+    <t>0.1uF/40V, Capacitor, Ceramic,  X7R, 5%</t>
+  </si>
+  <si>
+    <t>0.01uF, Capacitor, Ceramic,  X7R, 5%</t>
+  </si>
+  <si>
+    <t>0.047uF, Capacitor, Ceramic,  X7R, 5%</t>
+  </si>
+  <si>
+    <t>1n, Capacitor, Ceramic,  X7R, 5%</t>
+  </si>
+  <si>
+    <t>10nF, Capacitor, Ceramic,  X7R, 5%</t>
+  </si>
+  <si>
+    <t>100n/40V, Capacitor, Ceramic,  X7R, 5%</t>
+  </si>
+  <si>
+    <t>887-1819-1-ND</t>
+  </si>
+  <si>
+    <t>FERRITE CHIP 600 OHM 500MA</t>
+  </si>
+  <si>
+    <t>MMZ1608R601A</t>
+  </si>
+  <si>
+    <t>445-1547-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1149,8 +1164,8 @@
   <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,19 +1221,19 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E3" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="F3" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="G3" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="H3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I3" t="s">
         <v>80</v>
@@ -1232,22 +1247,22 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D4" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E4" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="F4" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="G4" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="H4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I4" t="s">
         <v>80</v>
@@ -1261,22 +1276,22 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D5" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E5" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="F5" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="H5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I5" t="s">
         <v>80</v>
@@ -1292,11 +1307,20 @@
       <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>107</v>
+      <c r="D6" t="s">
+        <v>234</v>
+      </c>
+      <c r="E6" t="s">
+        <v>242</v>
+      </c>
+      <c r="F6" t="s">
+        <v>243</v>
+      </c>
+      <c r="G6" t="s">
+        <v>244</v>
       </c>
       <c r="H6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I6" t="s">
         <v>80</v>
@@ -1313,16 +1337,19 @@
         <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="F7" t="s">
+        <v>254</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I7" t="s">
         <v>82</v>
@@ -1339,13 +1366,13 @@
         <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
@@ -1365,13 +1392,13 @@
         <v>77</v>
       </c>
       <c r="D9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="E9" t="s">
-        <v>112</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="H9" t="s">
         <v>12</v>
@@ -1391,16 +1418,16 @@
         <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I10" t="s">
         <v>82</v>
@@ -1417,19 +1444,19 @@
         <v>37</v>
       </c>
       <c r="D11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" t="s">
         <v>115</v>
-      </c>
-      <c r="E11" t="s">
-        <v>123</v>
-      </c>
-      <c r="F11" t="s">
-        <v>154</v>
-      </c>
-      <c r="G11" t="s">
-        <v>117</v>
-      </c>
-      <c r="H11" t="s">
-        <v>116</v>
       </c>
       <c r="I11" t="s">
         <v>82</v>
@@ -1446,16 +1473,16 @@
         <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
@@ -1475,19 +1502,19 @@
         <v>79</v>
       </c>
       <c r="D13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>203</v>
+        <v>248</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I13" t="s">
         <v>82</v>
@@ -1504,19 +1531,19 @@
         <v>81</v>
       </c>
       <c r="D14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>198</v>
+        <v>249</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I14" t="s">
         <v>82</v>
@@ -1533,19 +1560,19 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F15" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>197</v>
+        <v>250</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I15" t="s">
         <v>82</v>
@@ -1562,19 +1589,19 @@
         <v>83</v>
       </c>
       <c r="D16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>196</v>
+        <v>251</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I16" t="s">
         <v>82</v>
@@ -1591,19 +1618,19 @@
         <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I17" t="s">
         <v>82</v>
@@ -1620,19 +1647,19 @@
         <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>200</v>
+        <v>252</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I18" t="s">
         <v>82</v>
@@ -1649,19 +1676,19 @@
         <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F19" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>201</v>
+        <v>245</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I19" t="s">
         <v>82</v>
@@ -1678,19 +1705,19 @@
         <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>202</v>
+        <v>253</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I20" t="s">
         <v>82</v>
@@ -1707,19 +1734,19 @@
         <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E21" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F21" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>204</v>
+        <v>246</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I21" t="s">
         <v>82</v>
@@ -1736,19 +1763,19 @@
         <v>43</v>
       </c>
       <c r="D22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>205</v>
+        <v>247</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I22" t="s">
         <v>82</v>
@@ -1765,19 +1792,19 @@
         <v>86</v>
       </c>
       <c r="D23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I23" t="s">
         <v>82</v>
@@ -1794,19 +1821,19 @@
         <v>87</v>
       </c>
       <c r="D24" t="s">
+        <v>189</v>
+      </c>
+      <c r="E24" t="s">
+        <v>189</v>
+      </c>
+      <c r="F24" t="s">
+        <v>189</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="H24" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="E24" t="s">
-        <v>191</v>
-      </c>
-      <c r="F24" t="s">
-        <v>191</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="I24" t="s">
         <v>82</v>
@@ -1823,19 +1850,19 @@
         <v>88</v>
       </c>
       <c r="D25" t="s">
+        <v>189</v>
+      </c>
+      <c r="E25" t="s">
+        <v>189</v>
+      </c>
+      <c r="F25" t="s">
+        <v>189</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="E25" t="s">
-        <v>191</v>
-      </c>
-      <c r="F25" t="s">
-        <v>191</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="I25" t="s">
         <v>82</v>
@@ -1852,19 +1879,19 @@
         <v>89</v>
       </c>
       <c r="D26" t="s">
+        <v>189</v>
+      </c>
+      <c r="E26" t="s">
+        <v>189</v>
+      </c>
+      <c r="F26" t="s">
+        <v>189</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="E26" t="s">
-        <v>191</v>
-      </c>
-      <c r="F26" t="s">
-        <v>191</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="I26" t="s">
         <v>82</v>
@@ -1881,19 +1908,19 @@
         <v>44</v>
       </c>
       <c r="D27" t="s">
+        <v>189</v>
+      </c>
+      <c r="E27" t="s">
+        <v>189</v>
+      </c>
+      <c r="F27" t="s">
+        <v>189</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="E27" t="s">
-        <v>191</v>
-      </c>
-      <c r="F27" t="s">
-        <v>191</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="I27" t="s">
         <v>82</v>
@@ -1910,19 +1937,19 @@
         <v>45</v>
       </c>
       <c r="D28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I28" t="s">
         <v>82</v>
@@ -1939,19 +1966,19 @@
         <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F29" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I29" t="s">
         <v>82</v>
@@ -1968,19 +1995,19 @@
         <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F30" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I30" t="s">
         <v>82</v>
@@ -1994,22 +2021,22 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="D31" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E31" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="F31" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="G31" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I31" t="s">
         <v>82</v>
@@ -2023,22 +2050,22 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D32" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="E32" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="G32" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I32" t="s">
         <v>82</v>
@@ -2055,19 +2082,19 @@
         <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" t="s">
+        <v>166</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="F33" t="s">
-        <v>168</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>125</v>
-      </c>
       <c r="H33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I33" t="s">
         <v>82</v>
@@ -2084,19 +2111,19 @@
         <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E34" t="s">
         <v>75</v>
       </c>
       <c r="F34" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I34" t="s">
         <v>82</v>
@@ -2113,19 +2140,19 @@
         <v>48</v>
       </c>
       <c r="D35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E35" t="s">
         <v>16</v>
       </c>
       <c r="F35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I35" t="s">
         <v>82</v>
@@ -2141,11 +2168,20 @@
       <c r="C36" t="s">
         <v>49</v>
       </c>
-      <c r="G36" s="5" t="s">
-        <v>159</v>
+      <c r="D36" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" t="s">
+        <v>256</v>
+      </c>
+      <c r="F36" t="s">
+        <v>257</v>
+      </c>
+      <c r="G36" t="s">
+        <v>255</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I36" t="s">
         <v>82</v>
@@ -2162,16 +2198,16 @@
         <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="E37" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="F37" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="H37" t="s">
         <v>76</v>
@@ -2191,19 +2227,19 @@
         <v>92</v>
       </c>
       <c r="D38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E38" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F38" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I38" t="s">
         <v>82</v>
@@ -2217,22 +2253,22 @@
         <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D39" t="s">
+        <v>179</v>
+      </c>
+      <c r="E39" t="s">
+        <v>187</v>
+      </c>
+      <c r="F39" t="s">
+        <v>184</v>
+      </c>
+      <c r="G39" t="s">
         <v>181</v>
       </c>
-      <c r="E39" t="s">
-        <v>189</v>
-      </c>
-      <c r="F39" t="s">
-        <v>186</v>
-      </c>
-      <c r="G39" t="s">
-        <v>183</v>
-      </c>
       <c r="H39" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I39" t="s">
         <v>82</v>
@@ -2249,19 +2285,19 @@
         <v>93</v>
       </c>
       <c r="D40" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E40" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F40" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I40" t="s">
         <v>82</v>
@@ -2278,19 +2314,19 @@
         <v>51</v>
       </c>
       <c r="D41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F41" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G41" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H41" t="s">
         <v>130</v>
-      </c>
-      <c r="H41" t="s">
-        <v>131</v>
       </c>
       <c r="I41" t="s">
         <v>82</v>
@@ -2307,19 +2343,19 @@
         <v>94</v>
       </c>
       <c r="D42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E42" t="s">
         <v>18</v>
       </c>
       <c r="F42" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G42" t="s">
+        <v>158</v>
+      </c>
+      <c r="H42" t="s">
         <v>160</v>
-      </c>
-      <c r="H42" t="s">
-        <v>162</v>
       </c>
       <c r="I42" t="s">
         <v>82</v>
@@ -2336,19 +2372,19 @@
         <v>52</v>
       </c>
       <c r="D43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E43" t="s">
         <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G43" t="s">
+        <v>132</v>
+      </c>
+      <c r="H43" t="s">
         <v>133</v>
-      </c>
-      <c r="H43" t="s">
-        <v>134</v>
       </c>
       <c r="I43" t="s">
         <v>82</v>
@@ -2365,16 +2401,16 @@
         <v>95</v>
       </c>
       <c r="D44" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>20</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H44" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I44" t="s">
         <v>82</v>
@@ -2391,16 +2427,16 @@
         <v>96</v>
       </c>
       <c r="D45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E45" t="s">
         <v>21</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I45" t="s">
         <v>82</v>
@@ -2477,19 +2513,19 @@
         <v>98</v>
       </c>
       <c r="D49" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E49" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F49" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I49" t="s">
         <v>82</v>
@@ -2506,19 +2542,19 @@
         <v>55</v>
       </c>
       <c r="D50" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E50" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F50" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>25</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I50" t="s">
         <v>82</v>
@@ -2535,19 +2571,19 @@
         <v>56</v>
       </c>
       <c r="D51" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E51" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F51" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I51" t="s">
         <v>82</v>
@@ -2564,19 +2600,19 @@
         <v>99</v>
       </c>
       <c r="D52" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E52" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F52" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I52" t="s">
         <v>82</v>
@@ -2593,19 +2629,19 @@
         <v>100</v>
       </c>
       <c r="D53" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E53" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F53" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G53" s="5" t="s">
         <v>27</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I53" t="s">
         <v>82</v>
@@ -2622,19 +2658,19 @@
         <v>57</v>
       </c>
       <c r="D54" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E54" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F54" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>28</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I54" t="s">
         <v>82</v>
@@ -2651,19 +2687,19 @@
         <v>58</v>
       </c>
       <c r="D55" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E55" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F55" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>29</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I55" t="s">
         <v>82</v>
@@ -2680,19 +2716,19 @@
         <v>101</v>
       </c>
       <c r="D56" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E56" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F56" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I56" t="s">
         <v>82</v>
@@ -2706,22 +2742,22 @@
         <v>25</v>
       </c>
       <c r="C57" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="D57" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E57" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F57" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I57" t="s">
         <v>82</v>
@@ -2738,19 +2774,19 @@
         <v>59</v>
       </c>
       <c r="D58" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E58" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F58" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>30</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I58" t="s">
         <v>82</v>
@@ -2767,19 +2803,19 @@
         <v>102</v>
       </c>
       <c r="D59" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E59" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F59" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G59" s="5">
         <v>51</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I59" t="s">
         <v>82</v>
@@ -2796,19 +2832,19 @@
         <v>60</v>
       </c>
       <c r="D60" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E60" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F60" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I60" t="s">
         <v>82</v>
@@ -2825,19 +2861,19 @@
         <v>61</v>
       </c>
       <c r="D61" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E61" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F61" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G61" s="5">
         <v>100</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I61" t="s">
         <v>82</v>
@@ -2854,19 +2890,19 @@
         <v>62</v>
       </c>
       <c r="D62" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E62" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F62" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>31</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I62" t="s">
         <v>82</v>
@@ -2883,19 +2919,19 @@
         <v>63</v>
       </c>
       <c r="D63" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E63" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F63" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I63" t="s">
         <v>82</v>
@@ -2912,19 +2948,19 @@
         <v>64</v>
       </c>
       <c r="D64" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E64" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F64" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I64" t="s">
         <v>82</v>
@@ -2941,19 +2977,19 @@
         <v>65</v>
       </c>
       <c r="D65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F65" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I65" t="s">
         <v>82</v>
@@ -2970,19 +3006,19 @@
         <v>66</v>
       </c>
       <c r="D66" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E66" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F66" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I66" t="s">
         <v>82</v>
@@ -2999,19 +3035,19 @@
         <v>103</v>
       </c>
       <c r="D67" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E67" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F67" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G67" s="5">
         <v>750</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I67" t="s">
         <v>82</v>
@@ -3028,19 +3064,19 @@
         <v>104</v>
       </c>
       <c r="D68" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E68" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F68" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>15</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I68" t="s">
         <v>82</v>
@@ -3057,19 +3093,19 @@
         <v>67</v>
       </c>
       <c r="D69" t="s">
+        <v>189</v>
+      </c>
+      <c r="E69" t="s">
+        <v>189</v>
+      </c>
+      <c r="F69" t="s">
+        <v>189</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H69" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="E69" t="s">
-        <v>191</v>
-      </c>
-      <c r="F69" t="s">
-        <v>191</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="I69" t="s">
         <v>82</v>
@@ -3086,19 +3122,19 @@
         <v>68</v>
       </c>
       <c r="D70" t="s">
+        <v>189</v>
+      </c>
+      <c r="E70" t="s">
+        <v>189</v>
+      </c>
+      <c r="F70" t="s">
+        <v>189</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="H70" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="E70" t="s">
-        <v>191</v>
-      </c>
-      <c r="F70" t="s">
-        <v>191</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="I70" t="s">
         <v>82</v>
@@ -3115,19 +3151,19 @@
         <v>69</v>
       </c>
       <c r="D71" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="E71" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="F71" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="G71" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="I71" t="s">
         <v>82</v>
@@ -3144,19 +3180,19 @@
         <v>70</v>
       </c>
       <c r="D72" t="s">
+        <v>173</v>
+      </c>
+      <c r="E72" t="s">
+        <v>170</v>
+      </c>
+      <c r="F72" t="s">
         <v>175</v>
       </c>
-      <c r="E72" t="s">
+      <c r="G72" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="F72" t="s">
-        <v>177</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>174</v>
-      </c>
       <c r="H72" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I72" t="s">
         <v>82</v>
@@ -3173,19 +3209,19 @@
         <v>71</v>
       </c>
       <c r="D73" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E73" t="s">
+        <v>169</v>
+      </c>
+      <c r="F73" t="s">
+        <v>174</v>
+      </c>
+      <c r="G73" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="F73" t="s">
-        <v>176</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>173</v>
-      </c>
       <c r="H73" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I73" t="s">
         <v>82</v>
@@ -3202,19 +3238,19 @@
         <v>105</v>
       </c>
       <c r="D74" t="s">
+        <v>150</v>
+      </c>
+      <c r="E74" t="s">
+        <v>149</v>
+      </c>
+      <c r="F74" t="s">
+        <v>147</v>
+      </c>
+      <c r="G74" t="s">
         <v>151</v>
       </c>
-      <c r="E74" t="s">
-        <v>150</v>
-      </c>
-      <c r="F74" t="s">
+      <c r="H74" t="s">
         <v>148</v>
-      </c>
-      <c r="G74" t="s">
-        <v>152</v>
-      </c>
-      <c r="H74" t="s">
-        <v>149</v>
       </c>
       <c r="I74" t="s">
         <v>82</v>
@@ -3231,19 +3267,19 @@
         <v>72</v>
       </c>
       <c r="D75" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E75" t="s">
         <v>32</v>
       </c>
       <c r="F75" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G75" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H75" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I75" t="s">
         <v>82</v>
@@ -3260,13 +3296,13 @@
         <v>73</v>
       </c>
       <c r="D76" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>33</v>
       </c>
       <c r="G76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I76" t="s">
         <v>82</v>
@@ -3283,19 +3319,19 @@
         <v>74</v>
       </c>
       <c r="D77" t="s">
+        <v>135</v>
+      </c>
+      <c r="E77" t="s">
         <v>136</v>
       </c>
-      <c r="E77" t="s">
-        <v>137</v>
-      </c>
       <c r="F77" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G77" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H77" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I77" t="s">
         <v>82</v>
@@ -3312,19 +3348,19 @@
         <v>106</v>
       </c>
       <c r="D78" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E78" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F78" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G78" t="s">
+        <v>137</v>
+      </c>
+      <c r="H78" t="s">
         <v>138</v>
-      </c>
-      <c r="H78" t="s">
-        <v>139</v>
       </c>
       <c r="I78" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
Added USB port digikey part to bom
</commit_message>
<xml_diff>
--- a/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
+++ b/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="263">
   <si>
     <t>Item #</t>
   </si>
@@ -57,9 +57,6 @@
     <t>ALT4532</t>
   </si>
   <si>
-    <t>BAT54</t>
-  </si>
-  <si>
     <t>BSS138W-7-F</t>
   </si>
   <si>
@@ -357,9 +354,6 @@
     <t>ACM2012-900-2P-T002</t>
   </si>
   <si>
-    <t>30 V Schottky barrier (double) diodes</t>
-  </si>
-  <si>
     <t>Texas Instruments</t>
   </si>
   <si>
@@ -790,6 +784,27 @@
   </si>
   <si>
     <t>445-1547-1-ND</t>
+  </si>
+  <si>
+    <t>BAT54-V-G</t>
+  </si>
+  <si>
+    <t>Diode, Schottky, 200-mA, 30-V</t>
+  </si>
+  <si>
+    <t>BAT54-V-GS08CT-ND</t>
+  </si>
+  <si>
+    <t>BSS84CT-ND</t>
+  </si>
+  <si>
+    <t>Obsolete</t>
+  </si>
+  <si>
+    <t>296-35921-1-ND</t>
+  </si>
+  <si>
+    <t>SOT23-6</t>
   </si>
 </sst>
 </file>
@@ -1164,8 +1179,8 @@
   <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,22 +1236,22 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F3" t="s">
         <v>234</v>
       </c>
-      <c r="E3" t="s">
-        <v>237</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>236</v>
       </c>
-      <c r="G3" t="s">
-        <v>238</v>
-      </c>
       <c r="H3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1247,25 +1262,25 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F4" t="s">
+        <v>237</v>
+      </c>
+      <c r="G4" t="s">
         <v>239</v>
       </c>
-      <c r="G4" t="s">
-        <v>241</v>
-      </c>
       <c r="H4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1276,25 +1291,25 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F5" t="s">
+        <v>230</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="F5" t="s">
-        <v>232</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>235</v>
-      </c>
       <c r="H5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1305,25 +1320,25 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E6" t="s">
+        <v>240</v>
+      </c>
+      <c r="F6" t="s">
+        <v>241</v>
+      </c>
+      <c r="G6" t="s">
         <v>242</v>
       </c>
-      <c r="F6" t="s">
-        <v>243</v>
-      </c>
-      <c r="G6" t="s">
-        <v>244</v>
-      </c>
       <c r="H6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1334,25 +1349,25 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1363,22 +1378,22 @@
         <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H8" t="s">
         <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1389,22 +1404,22 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="E9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="H9" t="s">
         <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1415,22 +1430,25 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>256</v>
+      </c>
+      <c r="F10" t="s">
+        <v>258</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>113</v>
+        <v>257</v>
       </c>
       <c r="H10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1441,25 +1459,25 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G11" t="s">
         <v>114</v>
       </c>
-      <c r="E11" t="s">
-        <v>122</v>
-      </c>
-      <c r="F11" t="s">
-        <v>153</v>
-      </c>
-      <c r="G11" t="s">
-        <v>116</v>
-      </c>
       <c r="H11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1470,25 +1488,25 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1499,25 +1517,25 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F13" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1528,25 +1546,25 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1557,25 +1575,25 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F15" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1586,25 +1604,25 @@
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1615,25 +1633,25 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1644,25 +1662,25 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1673,25 +1691,25 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1702,25 +1720,25 @@
         <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1731,25 +1749,25 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1760,25 +1778,25 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1789,25 +1807,25 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1818,25 +1836,25 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" t="s">
+        <v>187</v>
+      </c>
+      <c r="E24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F24" t="s">
+        <v>187</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H24" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E24" t="s">
-        <v>189</v>
-      </c>
-      <c r="F24" t="s">
-        <v>189</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>191</v>
-      </c>
       <c r="I24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1847,25 +1865,25 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D25" t="s">
+        <v>187</v>
+      </c>
+      <c r="E25" t="s">
+        <v>187</v>
+      </c>
+      <c r="F25" t="s">
+        <v>187</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E25" t="s">
-        <v>189</v>
-      </c>
-      <c r="F25" t="s">
-        <v>189</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>191</v>
-      </c>
       <c r="I25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1876,25 +1894,25 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D26" t="s">
+        <v>187</v>
+      </c>
+      <c r="E26" t="s">
+        <v>187</v>
+      </c>
+      <c r="F26" t="s">
+        <v>187</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E26" t="s">
-        <v>189</v>
-      </c>
-      <c r="F26" t="s">
-        <v>189</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>191</v>
-      </c>
       <c r="I26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1905,25 +1923,25 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
+        <v>187</v>
+      </c>
+      <c r="E27" t="s">
+        <v>187</v>
+      </c>
+      <c r="F27" t="s">
+        <v>187</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E27" t="s">
-        <v>189</v>
-      </c>
-      <c r="F27" t="s">
-        <v>189</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>191</v>
-      </c>
       <c r="I27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1934,25 +1952,25 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E28" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F28" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1963,25 +1981,25 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -1992,25 +2010,25 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2021,25 +2039,25 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
+        <v>222</v>
+      </c>
+      <c r="D31" t="s">
+        <v>223</v>
+      </c>
+      <c r="E31" t="s">
         <v>224</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
         <v>225</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
         <v>226</v>
       </c>
-      <c r="F31" t="s">
-        <v>227</v>
-      </c>
-      <c r="G31" t="s">
-        <v>228</v>
-      </c>
       <c r="H31" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2050,25 +2068,25 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
+        <v>221</v>
+      </c>
+      <c r="D32" t="s">
         <v>223</v>
       </c>
-      <c r="D32" t="s">
-        <v>225</v>
-      </c>
       <c r="E32" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F32" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="G32" t="s">
         <v>229</v>
       </c>
-      <c r="G32" t="s">
-        <v>231</v>
-      </c>
       <c r="H32" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2079,25 +2097,25 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H33" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2108,25 +2126,25 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F34" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H34" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2137,25 +2155,25 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D35" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F35" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2166,25 +2184,25 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E36" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F36" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G36" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2195,25 +2213,25 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D37" t="s">
+        <v>200</v>
+      </c>
+      <c r="E37" t="s">
+        <v>201</v>
+      </c>
+      <c r="F37" t="s">
         <v>202</v>
       </c>
-      <c r="E37" t="s">
-        <v>203</v>
-      </c>
-      <c r="F37" t="s">
-        <v>204</v>
-      </c>
       <c r="G37" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2224,25 +2242,25 @@
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E38" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F38" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2253,25 +2271,25 @@
         <v>9</v>
       </c>
       <c r="C39" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D39" t="s">
+        <v>177</v>
+      </c>
+      <c r="E39" t="s">
+        <v>185</v>
+      </c>
+      <c r="F39" t="s">
+        <v>182</v>
+      </c>
+      <c r="G39" t="s">
         <v>179</v>
       </c>
-      <c r="E39" t="s">
-        <v>187</v>
-      </c>
-      <c r="F39" t="s">
-        <v>184</v>
-      </c>
-      <c r="G39" t="s">
-        <v>181</v>
-      </c>
       <c r="H39" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2282,25 +2300,25 @@
         <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D40" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E40" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F40" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G40" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2311,25 +2329,25 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D41" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" t="s">
+        <v>129</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H41" t="s">
         <v>128</v>
       </c>
-      <c r="E41" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F41" t="s">
-        <v>131</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="H41" t="s">
-        <v>130</v>
-      </c>
       <c r="I41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2340,25 +2358,25 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D42" t="s">
+        <v>157</v>
+      </c>
+      <c r="E42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" t="s">
         <v>159</v>
       </c>
-      <c r="E42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F42" t="s">
-        <v>161</v>
-      </c>
       <c r="G42" t="s">
+        <v>156</v>
+      </c>
+      <c r="H42" t="s">
         <v>158</v>
       </c>
-      <c r="H42" t="s">
-        <v>160</v>
-      </c>
       <c r="I42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2369,25 +2387,25 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D43" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F43" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2398,22 +2416,25 @@
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D44" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="F44" t="s">
+        <v>260</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2424,22 +2445,25 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D45" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E45" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="F45" t="s">
+        <v>259</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H45" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2450,16 +2474,16 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2470,16 +2494,16 @@
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2490,16 +2514,16 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2510,25 +2534,25 @@
         <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D49" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E49" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F49" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2539,25 +2563,25 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D50" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E50" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F50" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2568,25 +2592,25 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I51" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2597,25 +2621,25 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D52" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E52" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F52" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2626,25 +2650,25 @@
         <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D53" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E53" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F53" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2655,25 +2679,25 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D54" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E54" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F54" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2684,25 +2708,25 @@
         <v>1</v>
       </c>
       <c r="C55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D55" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E55" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F55" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2713,25 +2737,25 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D56" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E56" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F56" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I56" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2742,25 +2766,25 @@
         <v>25</v>
       </c>
       <c r="C57" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D57" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E57" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F57" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2771,25 +2795,25 @@
         <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D58" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E58" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F58" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2800,25 +2824,25 @@
         <v>48</v>
       </c>
       <c r="C59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D59" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E59" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F59" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G59" s="5">
         <v>51</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -2829,25 +2853,25 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E60" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F60" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I60" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2858,25 +2882,25 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D61" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E61" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F61" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G61" s="5">
         <v>100</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -2887,25 +2911,25 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D62" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E62" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F62" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I62" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -2916,25 +2940,25 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D63" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E63" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F63" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I63" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -2945,25 +2969,25 @@
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E64" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F64" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -2974,25 +2998,25 @@
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D65" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E65" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F65" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I65" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3003,25 +3027,25 @@
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D66" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E66" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F66" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I66" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3032,25 +3056,25 @@
         <v>27</v>
       </c>
       <c r="C67" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D67" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E67" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F67" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G67" s="5">
         <v>750</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3061,25 +3085,25 @@
         <v>21</v>
       </c>
       <c r="C68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D68" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E68" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F68" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3090,25 +3114,25 @@
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D69" t="s">
+        <v>187</v>
+      </c>
+      <c r="E69" t="s">
+        <v>187</v>
+      </c>
+      <c r="F69" t="s">
+        <v>187</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="H69" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E69" t="s">
-        <v>189</v>
-      </c>
-      <c r="F69" t="s">
-        <v>189</v>
-      </c>
-      <c r="G69" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>191</v>
-      </c>
       <c r="I69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3119,25 +3143,25 @@
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D70" t="s">
+        <v>187</v>
+      </c>
+      <c r="E70" t="s">
+        <v>187</v>
+      </c>
+      <c r="F70" t="s">
+        <v>187</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="H70" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E70" t="s">
-        <v>189</v>
-      </c>
-      <c r="F70" t="s">
-        <v>189</v>
-      </c>
-      <c r="G70" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="H70" s="6" t="s">
-        <v>191</v>
-      </c>
       <c r="I70" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3148,25 +3172,25 @@
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D71" t="s">
+        <v>218</v>
+      </c>
+      <c r="E71" t="s">
+        <v>217</v>
+      </c>
+      <c r="F71" t="s">
+        <v>216</v>
+      </c>
+      <c r="G71" t="s">
+        <v>219</v>
+      </c>
+      <c r="H71" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="E71" t="s">
-        <v>219</v>
-      </c>
-      <c r="F71" t="s">
-        <v>218</v>
-      </c>
-      <c r="G71" t="s">
-        <v>221</v>
-      </c>
-      <c r="H71" s="6" t="s">
-        <v>222</v>
-      </c>
       <c r="I71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3177,25 +3201,25 @@
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D72" t="s">
+        <v>171</v>
+      </c>
+      <c r="E72" t="s">
+        <v>168</v>
+      </c>
+      <c r="F72" t="s">
         <v>173</v>
       </c>
-      <c r="E72" t="s">
+      <c r="G72" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="F72" t="s">
-        <v>175</v>
-      </c>
-      <c r="G72" s="5" t="s">
-        <v>172</v>
-      </c>
       <c r="H72" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3206,25 +3230,25 @@
         <v>1</v>
       </c>
       <c r="C73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D73" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E73" t="s">
+        <v>167</v>
+      </c>
+      <c r="F73" t="s">
+        <v>172</v>
+      </c>
+      <c r="G73" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="F73" t="s">
-        <v>174</v>
-      </c>
-      <c r="G73" s="5" t="s">
-        <v>171</v>
-      </c>
       <c r="H73" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3235,25 +3259,25 @@
         <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D74" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E74" t="s">
+        <v>147</v>
+      </c>
+      <c r="F74" t="s">
+        <v>145</v>
+      </c>
+      <c r="G74" t="s">
         <v>149</v>
       </c>
-      <c r="F74" t="s">
-        <v>147</v>
-      </c>
-      <c r="G74" t="s">
-        <v>151</v>
-      </c>
       <c r="H74" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="I74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -3264,25 +3288,25 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D75" t="s">
+        <v>142</v>
+      </c>
+      <c r="E75" t="s">
+        <v>31</v>
+      </c>
+      <c r="F75" t="s">
         <v>144</v>
       </c>
-      <c r="E75" t="s">
-        <v>32</v>
-      </c>
-      <c r="F75" t="s">
-        <v>146</v>
-      </c>
       <c r="G75" t="s">
+        <v>141</v>
+      </c>
+      <c r="H75" t="s">
         <v>143</v>
       </c>
-      <c r="H75" t="s">
-        <v>145</v>
-      </c>
       <c r="I75" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -3293,19 +3317,25 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D76" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="F76" t="s">
+        <v>261</v>
       </c>
       <c r="G76" t="s">
-        <v>155</v>
+        <v>153</v>
+      </c>
+      <c r="H76" t="s">
+        <v>262</v>
       </c>
       <c r="I76" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3316,25 +3346,25 @@
         <v>1</v>
       </c>
       <c r="C77" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D77" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E77" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F77" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G77" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H77" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I77" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3345,25 +3375,25 @@
         <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D78" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E78" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F78" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G78" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H78" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I78" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added last of resistor part numbers, as required by SC.
</commit_message>
<xml_diff>
--- a/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
+++ b/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="368">
   <si>
     <t>Item #</t>
   </si>
@@ -492,9 +492,6 @@
     <t>APT1608SYCK</t>
   </si>
   <si>
-    <t>Std</t>
-  </si>
-  <si>
     <t>0402</t>
   </si>
   <si>
@@ -783,9 +780,6 @@
     <t>R49,R52,R54,R56,R58,R60,R62</t>
   </si>
   <si>
-    <t>std</t>
-  </si>
-  <si>
     <t>R51,R66,R67,R68,R69,R70,R71,R138</t>
   </si>
   <si>
@@ -993,9 +987,6 @@
     <t>Diode, Schottky, 500mA, 20V</t>
   </si>
   <si>
-    <t>PSAS Rocketnet Hub v1.0 PCB BOM for assembly at Screaming Circuits 2013/07/15</t>
-  </si>
-  <si>
     <t>Unique Parts</t>
   </si>
   <si>
@@ -1006,6 +997,129 @@
   </si>
   <si>
     <t>Fine pitch/leadless</t>
+  </si>
+  <si>
+    <t>541-7.50LLCT-ND</t>
+  </si>
+  <si>
+    <t>P10.0LCT-ND</t>
+  </si>
+  <si>
+    <t>P51.0LCT-ND</t>
+  </si>
+  <si>
+    <t>P100LCT-ND</t>
+  </si>
+  <si>
+    <t>P200LCT-ND</t>
+  </si>
+  <si>
+    <t>P1.00KLCT-ND</t>
+  </si>
+  <si>
+    <t>P2.20KLCT-ND</t>
+  </si>
+  <si>
+    <t>P1.20KLCT-ND</t>
+  </si>
+  <si>
+    <t>P4.02KLCT-ND</t>
+  </si>
+  <si>
+    <t>P49.9KLCT-ND</t>
+  </si>
+  <si>
+    <t>P66.5KLCT-ND</t>
+  </si>
+  <si>
+    <t>P69.8KLCT-ND</t>
+  </si>
+  <si>
+    <t>P80.6KLCT-ND</t>
+  </si>
+  <si>
+    <t>P100KLCT-ND</t>
+  </si>
+  <si>
+    <t>P154KLCT-ND</t>
+  </si>
+  <si>
+    <t>P316KLCT-ND</t>
+  </si>
+  <si>
+    <t>P430KLCT-ND</t>
+  </si>
+  <si>
+    <t>P1.00MLCT-ND</t>
+  </si>
+  <si>
+    <t>541-3.01MLCT-ND</t>
+  </si>
+  <si>
+    <t>445-8639-1-ND</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>CRCW04027R50FKED</t>
+  </si>
+  <si>
+    <t>CRCW04023M01FKED</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF10R0X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF51R0X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1000X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF2000X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1001X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1201X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF2201X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF4021X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF4992X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF6652X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF6982X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF8062X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1003X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1543X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF3163X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF4303X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1004X</t>
+  </si>
+  <si>
+    <t>PSAS Rocketnet Hub v1.0 PCB BOM for assembly at Screaming Circuits 2013/07/18</t>
   </si>
 </sst>
 </file>
@@ -1395,7 +1509,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I84" sqref="I84"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1413,7 +1527,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="7" customFormat="1">
       <c r="A1" s="7" t="s">
-        <v>325</v>
+        <v>367</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1456,19 +1570,19 @@
         <v>64</v>
       </c>
       <c r="D4" t="s">
+        <v>279</v>
+      </c>
+      <c r="E4" t="s">
         <v>281</v>
       </c>
-      <c r="E4" t="s">
-        <v>283</v>
-      </c>
       <c r="F4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I4" t="s">
         <v>62</v>
@@ -1486,19 +1600,19 @@
         <v>28</v>
       </c>
       <c r="D5" t="s">
+        <v>282</v>
+      </c>
+      <c r="E5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F5" t="s">
         <v>284</v>
       </c>
-      <c r="E5" t="s">
-        <v>285</v>
-      </c>
-      <c r="F5" t="s">
-        <v>286</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I5" t="s">
         <v>62</v>
@@ -1516,19 +1630,19 @@
         <v>63</v>
       </c>
       <c r="D6" t="s">
+        <v>285</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>289</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>62</v>
@@ -1546,19 +1660,19 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I7" t="s">
         <v>62</v>
@@ -1573,22 +1687,22 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I8" t="s">
         <v>62</v>
@@ -1606,19 +1720,19 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F9" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I9" t="s">
         <v>62</v>
@@ -1633,22 +1747,22 @@
         <v>50</v>
       </c>
       <c r="C10" t="s">
+        <v>295</v>
+      </c>
+      <c r="D10" t="s">
+        <v>285</v>
+      </c>
+      <c r="E10" t="s">
+        <v>296</v>
+      </c>
+      <c r="F10" t="s">
         <v>297</v>
       </c>
-      <c r="D10" t="s">
-        <v>287</v>
-      </c>
-      <c r="E10" t="s">
-        <v>298</v>
-      </c>
-      <c r="F10" t="s">
-        <v>299</v>
-      </c>
       <c r="G10" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I10" t="s">
         <v>62</v>
@@ -1666,19 +1780,19 @@
         <v>67</v>
       </c>
       <c r="D11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>62</v>
@@ -1693,22 +1807,22 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>300</v>
+      </c>
+      <c r="D12" t="s">
+        <v>301</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>305</v>
-      </c>
       <c r="G12" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>62</v>
@@ -1726,19 +1840,19 @@
         <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>62</v>
@@ -1756,19 +1870,19 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>62</v>
@@ -1786,19 +1900,19 @@
         <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E15" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>309</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>312</v>
-      </c>
       <c r="H15" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>62</v>
@@ -1816,19 +1930,19 @@
         <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I16" s="8" t="s">
         <v>62</v>
@@ -1846,19 +1960,19 @@
         <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>62</v>
@@ -1876,19 +1990,19 @@
         <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I18" s="8" t="s">
         <v>62</v>
@@ -1906,19 +2020,19 @@
         <v>69</v>
       </c>
       <c r="D19" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E19" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F19" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I19" t="s">
         <v>62</v>
@@ -1939,13 +2053,13 @@
         <v>100</v>
       </c>
       <c r="E20" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>211</v>
-      </c>
       <c r="G20" s="4" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>92</v>
@@ -1963,19 +2077,19 @@
         <v>1</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>100</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G21" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>92</v>
@@ -1993,22 +2107,22 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>191</v>
-      </c>
       <c r="G22" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I22" s="8" t="s">
         <v>62</v>
@@ -2035,7 +2149,7 @@
         <v>120</v>
       </c>
       <c r="G23" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>119</v>
@@ -2059,16 +2173,16 @@
         <v>85</v>
       </c>
       <c r="E24" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>209</v>
-      </c>
       <c r="G24" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>62</v>
@@ -2086,19 +2200,19 @@
         <v>74</v>
       </c>
       <c r="D25" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>230</v>
-      </c>
       <c r="F25" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I25" s="8" t="s">
         <v>61</v>
@@ -2116,16 +2230,16 @@
         <v>145</v>
       </c>
       <c r="D26" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>195</v>
       </c>
       <c r="H26" s="8" t="s">
         <v>94</v>
@@ -2146,19 +2260,19 @@
         <v>39</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>18</v>
       </c>
       <c r="H27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>61</v>
@@ -2176,16 +2290,16 @@
         <v>146</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>201</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>94</v>
@@ -2206,16 +2320,16 @@
         <v>9</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E29" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="G29" s="8" t="s">
         <v>197</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>198</v>
       </c>
       <c r="H29" s="8" t="s">
         <v>94</v>
@@ -2236,19 +2350,19 @@
         <v>40</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I30" s="8" t="s">
         <v>61</v>
@@ -2266,16 +2380,16 @@
         <v>23</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E31" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="G31" s="8" t="s">
         <v>203</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>204</v>
       </c>
       <c r="H31" s="8" t="s">
         <v>94</v>
@@ -2302,7 +2416,7 @@
         <v>58</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>101</v>
@@ -2332,7 +2446,7 @@
         <v>88</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G33" s="9" t="s">
         <v>84</v>
@@ -2368,7 +2482,7 @@
         <v>150</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I34" s="8" t="s">
         <v>62</v>
@@ -2398,7 +2512,7 @@
         <v>151</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I35" s="8" t="s">
         <v>62</v>
@@ -2428,7 +2542,7 @@
         <v>149</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>62</v>
@@ -2446,16 +2560,16 @@
         <v>36</v>
       </c>
       <c r="D37" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E37" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="F37" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="F37" s="8" t="s">
-        <v>171</v>
-      </c>
       <c r="G37" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>59</v>
@@ -2488,7 +2602,7 @@
         <v>95</v>
       </c>
       <c r="H38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>62</v>
@@ -2533,19 +2647,19 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D40" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="E40" t="s">
+        <v>216</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="G40" s="9" t="s">
         <v>219</v>
-      </c>
-      <c r="E40" t="s">
-        <v>217</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>220</v>
       </c>
       <c r="H40" s="8" t="s">
         <v>92</v>
@@ -2563,19 +2677,19 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
+        <v>221</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="E41" t="s">
         <v>223</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="G41" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>226</v>
       </c>
       <c r="H41" s="8" t="s">
         <v>92</v>
@@ -2611,7 +2725,7 @@
         <v>122</v>
       </c>
       <c r="I42" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2626,19 +2740,19 @@
         <v>75</v>
       </c>
       <c r="D43" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I43" s="8" t="s">
         <v>62</v>
@@ -2665,10 +2779,10 @@
         <v>144</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I44" s="8" t="s">
         <v>62</v>
@@ -2695,10 +2809,10 @@
         <v>143</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I45" s="8" t="s">
         <v>62</v>
@@ -2716,19 +2830,19 @@
         <v>52</v>
       </c>
       <c r="D46" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="G46" t="s">
+        <v>250</v>
+      </c>
+      <c r="H46" s="10" t="s">
         <v>187</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="G46" t="s">
-        <v>251</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>188</v>
       </c>
       <c r="I46" s="8" t="s">
         <v>62</v>
@@ -2746,19 +2860,19 @@
         <v>50</v>
       </c>
       <c r="D47" t="s">
-        <v>124</v>
+        <v>347</v>
       </c>
       <c r="E47" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="H47" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I47" s="8" t="s">
         <v>62</v>
@@ -2776,19 +2890,19 @@
         <v>51</v>
       </c>
       <c r="D48" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E48" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="H48" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F48" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I48" s="8" t="s">
         <v>62</v>
@@ -2806,19 +2920,19 @@
         <v>79</v>
       </c>
       <c r="D49" t="s">
-        <v>246</v>
-      </c>
-      <c r="E49" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E49" t="s">
+        <v>351</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="H49" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="H49" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>62</v>
@@ -2833,22 +2947,22 @@
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D50" t="s">
-        <v>246</v>
-      </c>
-      <c r="E50" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E50" t="s">
+        <v>352</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="H50" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I50" s="8" t="s">
         <v>62</v>
@@ -2863,22 +2977,22 @@
         <v>1</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D51" t="s">
-        <v>246</v>
-      </c>
-      <c r="E51" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E51" t="s">
+        <v>353</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="H51" s="13" t="s">
         <v>158</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="H51" s="13" t="s">
-        <v>159</v>
       </c>
       <c r="I51" s="8" t="s">
         <v>62</v>
@@ -2896,19 +3010,19 @@
         <v>80</v>
       </c>
       <c r="D52" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I52" s="8" t="s">
         <v>62</v>
@@ -2926,19 +3040,19 @@
         <v>76</v>
       </c>
       <c r="D53" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E53" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="H53" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="H53" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I53" s="8" t="s">
         <v>62</v>
@@ -2956,19 +3070,19 @@
         <v>41</v>
       </c>
       <c r="D54" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E54" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="F54" t="s">
+        <v>334</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="H54" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G54" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I54" s="8" t="s">
         <v>62</v>
@@ -2986,19 +3100,19 @@
         <v>77</v>
       </c>
       <c r="D55" t="s">
-        <v>246</v>
-      </c>
-      <c r="E55" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E55" t="s">
+        <v>356</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="H55" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F55" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G55" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="H55" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I55" s="8" t="s">
         <v>62</v>
@@ -3016,19 +3130,19 @@
         <v>44</v>
       </c>
       <c r="D56" t="s">
-        <v>246</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>250</v>
+        <v>245</v>
+      </c>
+      <c r="E56" t="s">
+        <v>249</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I56" s="8" t="s">
         <v>62</v>
@@ -3046,19 +3160,19 @@
         <v>78</v>
       </c>
       <c r="D57" t="s">
-        <v>246</v>
-      </c>
-      <c r="E57" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E57" t="s">
+        <v>357</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="G57" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="H57" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F57" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="H57" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I57" s="8" t="s">
         <v>62</v>
@@ -3073,22 +3187,22 @@
         <v>25</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D58" t="s">
+        <v>245</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="F58" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="E58" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>247</v>
-      </c>
       <c r="G58" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I58" s="8" t="s">
         <v>62</v>
@@ -3106,19 +3220,19 @@
         <v>45</v>
       </c>
       <c r="D59" t="s">
-        <v>246</v>
-      </c>
-      <c r="E59" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E59" t="s">
+        <v>358</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="H59" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="H59" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I59" s="8" t="s">
         <v>62</v>
@@ -3133,22 +3247,22 @@
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D60" t="s">
-        <v>246</v>
-      </c>
-      <c r="E60" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E60" t="s">
+        <v>359</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H60" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="H60" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I60" s="8" t="s">
         <v>62</v>
@@ -3163,22 +3277,22 @@
         <v>7</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D61" t="s">
-        <v>246</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>255</v>
+        <v>245</v>
+      </c>
+      <c r="E61" t="s">
+        <v>360</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>255</v>
+        <v>338</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I61" s="8" t="s">
         <v>62</v>
@@ -3193,22 +3307,22 @@
         <v>7</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D62" t="s">
-        <v>246</v>
-      </c>
-      <c r="E62" s="8" t="s">
-        <v>255</v>
+        <v>245</v>
+      </c>
+      <c r="E62" t="s">
+        <v>361</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>255</v>
+        <v>339</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I62" s="8" t="s">
         <v>62</v>
@@ -3226,19 +3340,19 @@
         <v>46</v>
       </c>
       <c r="D63" t="s">
-        <v>246</v>
-      </c>
-      <c r="E63" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E63" t="s">
+        <v>362</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H63" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F63" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G63" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="H63" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I63" s="8" t="s">
         <v>62</v>
@@ -3256,19 +3370,19 @@
         <v>47</v>
       </c>
       <c r="D64" t="s">
-        <v>246</v>
-      </c>
-      <c r="E64" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E64" t="s">
+        <v>363</v>
+      </c>
+      <c r="F64" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H64" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G64" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="H64" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I64" s="8" t="s">
         <v>62</v>
@@ -3286,19 +3400,19 @@
         <v>48</v>
       </c>
       <c r="D65" t="s">
-        <v>246</v>
-      </c>
-      <c r="E65" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E65" t="s">
+        <v>364</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="H65" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G65" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="H65" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I65" s="8" t="s">
         <v>62</v>
@@ -3316,19 +3430,19 @@
         <v>49</v>
       </c>
       <c r="D66" t="s">
-        <v>246</v>
-      </c>
-      <c r="E66" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E66" t="s">
+        <v>365</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H66" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F66" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G66" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="H66" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I66" s="8" t="s">
         <v>62</v>
@@ -3346,19 +3460,19 @@
         <v>42</v>
       </c>
       <c r="D67" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E67" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H67" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="H67" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I67" s="8" t="s">
         <v>62</v>
@@ -3376,19 +3490,19 @@
         <v>43</v>
       </c>
       <c r="D68" t="s">
-        <v>124</v>
+        <v>347</v>
       </c>
       <c r="E68" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="H68" s="11" t="s">
         <v>158</v>
-      </c>
-      <c r="F68" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="H68" s="11" t="s">
-        <v>159</v>
       </c>
       <c r="I68" s="8" t="s">
         <v>62</v>
@@ -3403,7 +3517,7 @@
         <v>16</v>
       </c>
       <c r="C69" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D69" s="8" t="s">
         <v>85</v>
@@ -3411,7 +3525,9 @@
       <c r="E69" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F69" s="8"/>
+      <c r="F69" s="8" t="s">
+        <v>346</v>
+      </c>
       <c r="G69" s="9" t="s">
         <v>86</v>
       </c>
@@ -3449,7 +3565,7 @@
         <v>90</v>
       </c>
       <c r="I70" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -3509,7 +3625,7 @@
         <v>105</v>
       </c>
       <c r="I72" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3539,7 +3655,7 @@
         <v>134</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3590,13 +3706,13 @@
         <v>22</v>
       </c>
       <c r="F75" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G75" s="8" t="s">
         <v>129</v>
       </c>
       <c r="H75" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I75" s="8" t="s">
         <v>62</v>
@@ -3659,7 +3775,7 @@
         <v>113</v>
       </c>
       <c r="I77" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3671,7 +3787,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>130</v>
@@ -3680,7 +3796,7 @@
         <v>83</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G78" s="9" t="s">
         <v>10</v>
@@ -3701,7 +3817,7 @@
     <row r="81" spans="7:9">
       <c r="G81" s="4"/>
       <c r="H81" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I81">
         <v>75</v>
@@ -3710,7 +3826,7 @@
     <row r="82" spans="7:9">
       <c r="G82" s="4"/>
       <c r="H82" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="I82">
         <f>SUMIF($I4:$I78,"smt",$B$4:$B$78)</f>
@@ -3720,7 +3836,7 @@
     <row r="83" spans="7:9">
       <c r="G83" s="4"/>
       <c r="H83" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="I83">
         <f>SUMIF($I5:$I79,"thru-hole",$B$4:$B$78)</f>
@@ -3730,7 +3846,7 @@
     <row r="84" spans="7:9">
       <c r="G84" s="4"/>
       <c r="H84" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="I84">
         <f>SUMIF($I6:$I80,"leadless",$B$4:$B$78)</f>

</xml_diff>

<commit_message>
Updated L1 Mfg part number.
</commit_message>
<xml_diff>
--- a/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
+++ b/av3/rocketnet-hub/Documentation/BOM_sc.xlsx
@@ -192,9 +192,6 @@
     <t>U1</t>
   </si>
   <si>
-    <t>IHLP-2525CZ-01</t>
-  </si>
-  <si>
     <t>LED_RGB_PLCC-6</t>
   </si>
   <si>
@@ -1120,6 +1117,9 @@
   </si>
   <si>
     <t>PSAS Rocketnet Hub v1.0 PCB BOM for assembly at Screaming Circuits 2013/07/18</t>
+  </si>
+  <si>
+    <t>IHLP2525CZER4R7M01</t>
   </si>
 </sst>
 </file>
@@ -1509,7 +1509,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1527,7 +1527,7 @@
   <sheetData>
     <row r="1" spans="1:9" s="7" customFormat="1">
       <c r="A1" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1567,25 +1567,25 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E4" t="s">
+        <v>280</v>
+      </c>
+      <c r="F4" t="s">
         <v>279</v>
       </c>
-      <c r="E4" t="s">
-        <v>281</v>
-      </c>
-      <c r="F4" t="s">
-        <v>280</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1">
@@ -1600,22 +1600,22 @@
         <v>28</v>
       </c>
       <c r="D5" t="s">
+        <v>281</v>
+      </c>
+      <c r="E5" t="s">
         <v>282</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>283</v>
       </c>
-      <c r="F5" t="s">
-        <v>284</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1627,25 +1627,25 @@
         <v>32</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" t="s">
+        <v>284</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>285</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="F6" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>287</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1660,22 +1660,22 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1687,25 +1687,25 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1720,22 +1720,22 @@
         <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E9" t="s">
+        <v>292</v>
+      </c>
+      <c r="F9" t="s">
         <v>293</v>
       </c>
-      <c r="F9" t="s">
-        <v>294</v>
-      </c>
       <c r="G9" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1747,25 +1747,25 @@
         <v>50</v>
       </c>
       <c r="C10" t="s">
+        <v>294</v>
+      </c>
+      <c r="D10" t="s">
+        <v>284</v>
+      </c>
+      <c r="E10" t="s">
         <v>295</v>
       </c>
-      <c r="D10" t="s">
-        <v>285</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>296</v>
       </c>
-      <c r="F10" t="s">
-        <v>297</v>
-      </c>
       <c r="G10" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1777,25 +1777,25 @@
         <v>7</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E11" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>299</v>
-      </c>
       <c r="G11" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1807,25 +1807,25 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
+        <v>299</v>
+      </c>
+      <c r="D12" t="s">
         <v>300</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="F12" s="8" t="s">
         <v>302</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>303</v>
-      </c>
       <c r="G12" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1837,25 +1837,25 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E13" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>305</v>
-      </c>
       <c r="G13" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1870,22 +1870,22 @@
         <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E14" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="F14" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>307</v>
-      </c>
       <c r="G14" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1897,25 +1897,25 @@
         <v>7</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E15" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="G15" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>310</v>
-      </c>
       <c r="H15" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1930,22 +1930,22 @@
         <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E16" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>312</v>
-      </c>
       <c r="G16" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1960,22 +1960,22 @@
         <v>32</v>
       </c>
       <c r="D17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E17" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>314</v>
-      </c>
       <c r="G17" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1987,25 +1987,25 @@
         <v>6</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E18" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="F18" s="8" t="s">
-        <v>316</v>
-      </c>
       <c r="G18" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -2017,25 +2017,25 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E19" t="s">
+        <v>316</v>
+      </c>
+      <c r="F19" t="s">
         <v>317</v>
       </c>
-      <c r="F19" t="s">
-        <v>318</v>
-      </c>
       <c r="G19" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -2050,22 +2050,22 @@
         <v>24</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E20" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>210</v>
-      </c>
       <c r="G20" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -2077,25 +2077,25 @@
         <v>1</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>239</v>
-      </c>
       <c r="G21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2107,25 +2107,25 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D22" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>190</v>
-      </c>
       <c r="G22" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2140,22 +2140,22 @@
         <v>55</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2170,22 +2170,22 @@
         <v>35</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E24" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>208</v>
-      </c>
       <c r="G24" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2197,25 +2197,25 @@
         <v>7</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>229</v>
-      </c>
       <c r="F25" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2227,25 +2227,25 @@
         <v>3</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D26" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="E26" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>194</v>
-      </c>
       <c r="H26" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2260,22 +2260,22 @@
         <v>39</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>18</v>
       </c>
       <c r="H27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2287,25 +2287,25 @@
         <v>8</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E28" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="G28" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>200</v>
-      </c>
       <c r="H28" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2320,22 +2320,22 @@
         <v>9</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E29" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="G29" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F29" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>197</v>
-      </c>
       <c r="H29" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -2350,22 +2350,22 @@
         <v>40</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E30" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2380,22 +2380,22 @@
         <v>23</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E31" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="G31" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="G31" s="8" t="s">
-        <v>203</v>
-      </c>
       <c r="H31" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -2410,22 +2410,22 @@
         <v>33</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>58</v>
+        <v>367</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -2437,25 +2437,25 @@
         <v>16</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H33" s="8" t="s">
         <v>11</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -2467,25 +2467,25 @@
         <v>9</v>
       </c>
       <c r="C34" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>148</v>
-      </c>
       <c r="E34" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2497,25 +2497,25 @@
         <v>7</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -2527,25 +2527,25 @@
         <v>9</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D36" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G36" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>149</v>
-      </c>
       <c r="H36" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2560,22 +2560,22 @@
         <v>36</v>
       </c>
       <c r="D37" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="E37" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="F37" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="F37" s="8" t="s">
-        <v>170</v>
-      </c>
       <c r="G37" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -2590,22 +2590,22 @@
         <v>26</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H38" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -2617,25 +2617,25 @@
         <v>3</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E39" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G39" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F39" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>99</v>
-      </c>
       <c r="H39" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2647,25 +2647,25 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D40" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="E40" t="s">
+        <v>215</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G40" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="E40" t="s">
-        <v>216</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>219</v>
-      </c>
       <c r="H40" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -2677,25 +2677,25 @@
         <v>2</v>
       </c>
       <c r="C41" t="s">
+        <v>220</v>
+      </c>
+      <c r="D41" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="E41" t="s">
         <v>222</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="F41" s="8" t="s">
+      <c r="G41" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="G41" s="8" t="s">
-        <v>225</v>
-      </c>
       <c r="H41" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -2707,25 +2707,25 @@
         <v>2</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D42" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G42" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="E42" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="F42" s="8" t="s">
+      <c r="H42" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G42" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="H42" s="8" t="s">
-        <v>122</v>
-      </c>
       <c r="I42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -2737,25 +2737,25 @@
         <v>13</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D43" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -2770,22 +2770,22 @@
         <v>53</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -2800,22 +2800,22 @@
         <v>54</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -2830,22 +2830,22 @@
         <v>52</v>
       </c>
       <c r="D46" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="G46" t="s">
+        <v>249</v>
+      </c>
+      <c r="H46" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="E46" s="8" t="s">
-        <v>185</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="G46" t="s">
-        <v>250</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>187</v>
-      </c>
       <c r="I46" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2860,22 +2860,22 @@
         <v>50</v>
       </c>
       <c r="D47" t="s">
+        <v>346</v>
+      </c>
+      <c r="E47" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="E47" s="8" t="s">
-        <v>348</v>
-      </c>
       <c r="F47" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2890,22 +2890,22 @@
         <v>51</v>
       </c>
       <c r="D48" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2917,25 +2917,25 @@
         <v>48</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D49" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E49" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2947,25 +2947,25 @@
         <v>2</v>
       </c>
       <c r="C50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D50" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E50" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2977,25 +2977,25 @@
         <v>1</v>
       </c>
       <c r="C51" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D51" t="s">
+        <v>244</v>
+      </c>
+      <c r="E51" t="s">
+        <v>352</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="G51" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="D51" t="s">
-        <v>245</v>
-      </c>
-      <c r="E51" t="s">
-        <v>353</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>270</v>
-      </c>
       <c r="H51" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -3007,25 +3007,25 @@
         <v>27</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D52" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -3037,25 +3037,25 @@
         <v>3</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D53" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -3070,22 +3070,22 @@
         <v>41</v>
       </c>
       <c r="D54" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F54" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -3097,25 +3097,25 @@
         <v>2</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D55" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E55" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -3130,22 +3130,22 @@
         <v>44</v>
       </c>
       <c r="D56" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E56" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -3157,25 +3157,25 @@
         <v>3</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D57" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E57" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -3187,25 +3187,25 @@
         <v>25</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D58" t="s">
+        <v>244</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="F58" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="E58" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="F58" s="8" t="s">
-        <v>246</v>
-      </c>
       <c r="G58" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -3220,22 +3220,22 @@
         <v>45</v>
       </c>
       <c r="D59" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E59" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H59" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -3247,25 +3247,25 @@
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D60" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E60" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -3277,25 +3277,25 @@
         <v>7</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D61" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E61" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -3307,25 +3307,25 @@
         <v>7</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D62" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E62" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H62" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -3340,22 +3340,22 @@
         <v>46</v>
       </c>
       <c r="D63" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E63" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I63" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -3370,22 +3370,22 @@
         <v>47</v>
       </c>
       <c r="D64" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E64" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -3400,22 +3400,22 @@
         <v>48</v>
       </c>
       <c r="D65" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E65" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -3430,22 +3430,22 @@
         <v>49</v>
       </c>
       <c r="D66" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E66" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F66" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -3460,22 +3460,22 @@
         <v>42</v>
       </c>
       <c r="D67" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F67" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H67" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -3490,22 +3490,22 @@
         <v>43</v>
       </c>
       <c r="D68" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E68" s="8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I68" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -3517,25 +3517,25 @@
         <v>16</v>
       </c>
       <c r="C69" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D69" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E69" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F69" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="G69" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F69" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="G69" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="H69" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I69" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -3550,22 +3550,22 @@
         <v>25</v>
       </c>
       <c r="D70" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E70" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H70" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E70" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F70" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H70" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="I70" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -3580,22 +3580,22 @@
         <v>34</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I71" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -3610,22 +3610,22 @@
         <v>37</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E72" s="9" t="s">
         <v>15</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G72" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H72" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="H72" s="8" t="s">
-        <v>105</v>
-      </c>
       <c r="I72" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -3637,25 +3637,25 @@
         <v>2</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H73" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I73" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -3670,22 +3670,22 @@
         <v>38</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G74" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H74" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="H74" s="8" t="s">
-        <v>108</v>
-      </c>
       <c r="I74" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -3700,22 +3700,22 @@
         <v>56</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E75" s="9" t="s">
         <v>22</v>
       </c>
       <c r="F75" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H75" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="G75" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="H75" s="8" t="s">
-        <v>212</v>
-      </c>
       <c r="I75" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -3730,22 +3730,22 @@
         <v>57</v>
       </c>
       <c r="D76" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E76" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E76" s="8" t="s">
-        <v>111</v>
-      </c>
       <c r="F76" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H76" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I76" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -3757,25 +3757,25 @@
         <v>7</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G77" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="H77" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H77" s="8" t="s">
-        <v>113</v>
-      </c>
       <c r="I77" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -3787,25 +3787,25 @@
         <v>1</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D78" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G78" s="9" t="s">
         <v>10</v>
       </c>
       <c r="H78" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I78" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -3817,7 +3817,7 @@
     <row r="81" spans="7:9">
       <c r="G81" s="4"/>
       <c r="H81" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I81">
         <v>75</v>
@@ -3826,7 +3826,7 @@
     <row r="82" spans="7:9">
       <c r="G82" s="4"/>
       <c r="H82" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I82">
         <f>SUMIF($I4:$I78,"smt",$B$4:$B$78)</f>
@@ -3836,7 +3836,7 @@
     <row r="83" spans="7:9">
       <c r="G83" s="4"/>
       <c r="H83" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I83">
         <f>SUMIF($I5:$I79,"thru-hole",$B$4:$B$78)</f>
@@ -3846,7 +3846,7 @@
     <row r="84" spans="7:9">
       <c r="G84" s="4"/>
       <c r="H84" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I84">
         <f>SUMIF($I6:$I80,"leadless",$B$4:$B$78)</f>

</xml_diff>